<commit_message>
add more details and update my progress
</commit_message>
<xml_diff>
--- a/TOEFL/Progress.xlsx
+++ b/TOEFL/Progress.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="3510" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="5850" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Progree" sheetId="1" r:id="rId1"/>
+    <sheet name="TPO Results" sheetId="4" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="36">
   <si>
     <t>Book/CD Name</t>
   </si>
@@ -51,9 +52,6 @@
     <t>ETS Essential Guide for TOEFL</t>
   </si>
   <si>
-    <t>TPO Tests</t>
-  </si>
-  <si>
     <t>TED Talks</t>
   </si>
   <si>
@@ -106,6 +104,30 @@
   </si>
   <si>
     <t>Notefull Videos and Docs / Writing</t>
+  </si>
+  <si>
+    <t>TPO Tests / Reading</t>
+  </si>
+  <si>
+    <t>TPO Tests / Listening</t>
+  </si>
+  <si>
+    <t>TPO Tests / Speaking</t>
+  </si>
+  <si>
+    <t>TPO Tests / Writing</t>
+  </si>
+  <si>
+    <t>AVG</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Hint= 20 is  the defult grade</t>
+  </si>
+  <si>
+    <t>Oxford English Grammar Course Book Tests</t>
   </si>
 </sst>
 </file>
@@ -172,7 +194,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -199,11 +221,66 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="12">
+  <dxfs count="20">
+    <dxf>
+      <font>
+        <b val="0"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -255,21 +332,38 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A2:J18" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="A2:J18"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A2:J22" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18">
+  <autoFilter ref="A2:J22"/>
   <tableColumns count="10">
-    <tableColumn id="1" name="No." dataDxfId="9"/>
-    <tableColumn id="2" name="Book/CD Name" dataDxfId="8"/>
-    <tableColumn id="3" name="Part/Page count" dataDxfId="7"/>
-    <tableColumn id="4" name="Current Part/Page" dataDxfId="6"/>
-    <tableColumn id="5" name="Progress" dataDxfId="5">
+    <tableColumn id="1" name="No." dataDxfId="17"/>
+    <tableColumn id="2" name="Book/CD Name" dataDxfId="16"/>
+    <tableColumn id="3" name="Part/Page count" dataDxfId="15"/>
+    <tableColumn id="4" name="Current Part/Page" dataDxfId="14"/>
+    <tableColumn id="5" name="Progress" dataDxfId="13">
       <calculatedColumnFormula xml:space="preserve"> CONCATENATE(CEILING(Table1[[#This Row],[Current Part/Page]]/Table1[[#This Row],[Part/Page count]], 0.0001) * 100,"%")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Reading" dataDxfId="4"/>
+    <tableColumn id="6" name="Reading" dataDxfId="12"/>
+    <tableColumn id="10" name="Listening" dataDxfId="11"/>
+    <tableColumn id="9" name="Speaking" dataDxfId="10"/>
+    <tableColumn id="8" name="Writing" dataDxfId="9"/>
+    <tableColumn id="12" name="Needs to be repeated" dataDxfId="8"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13" displayName="Table13" ref="A1:F56" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+  <autoFilter ref="A1:F56"/>
+  <tableColumns count="6">
+    <tableColumn id="1" name="No." dataDxfId="5"/>
+    <tableColumn id="6" name="Reading" dataDxfId="4">
+      <calculatedColumnFormula>aver</calculatedColumnFormula>
+    </tableColumn>
     <tableColumn id="10" name="Listening" dataDxfId="3"/>
     <tableColumn id="9" name="Speaking" dataDxfId="2"/>
     <tableColumn id="8" name="Writing" dataDxfId="1"/>
-    <tableColumn id="12" name="Needs to be repeated" dataDxfId="0"/>
+    <tableColumn id="12" name="Total" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -538,10 +632,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J21"/>
+  <dimension ref="A1:J25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -559,7 +653,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F1" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G1" s="9"/>
       <c r="H1" s="9"/>
@@ -582,19 +676,19 @@
         <v>4</v>
       </c>
       <c r="F2" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="G2" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="H2" s="6" t="s">
+      <c r="I2" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="I2" s="6" t="s">
-        <v>19</v>
-      </c>
       <c r="J2" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:10" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -615,16 +709,16 @@
         <v>12.36%</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J3" s="3">
         <v>1.5</v>
@@ -641,20 +735,20 @@
         <v>310</v>
       </c>
       <c r="D4" s="1">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="E4" s="5" t="str">
         <f xml:space="preserve"> CONCATENATE(CEILING(Table1[[#This Row],[Current Part/Page]]/Table1[[#This Row],[Part/Page count]], 0.0001) * 100,"%")</f>
-        <v>4.2%</v>
+        <v>5.17%</v>
       </c>
       <c r="F4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I4" s="3" t="s">
         <v>20</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>21</v>
       </c>
       <c r="J4" s="3"/>
     </row>
@@ -663,7 +757,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C5" s="1">
         <v>22</v>
@@ -673,115 +767,117 @@
         <v>0%</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J5" s="3"/>
     </row>
-    <row r="6" spans="1:10" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
+    <row r="6" spans="1:10" s="12" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="12">
         <v>4</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" s="1">
+      <c r="B6" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="C6" s="12">
         <v>17</v>
       </c>
-      <c r="E6" s="5" t="str">
+      <c r="E6" s="14" t="str">
         <f xml:space="preserve"> CONCATENATE(CEILING(Table1[[#This Row],[Current Part/Page]]/Table1[[#This Row],[Part/Page count]], 0.0001) * 100,"%")</f>
         <v>0%</v>
       </c>
-      <c r="F6" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="J6" s="3"/>
+      <c r="I6" s="13"/>
+      <c r="J6" s="13"/>
     </row>
     <row r="7" spans="1:10" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
+      <c r="A7" s="12">
         <v>5</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>7</v>
+      <c r="B7" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="C7" s="1">
-        <v>504</v>
+        <v>17</v>
       </c>
       <c r="E7" s="5" t="str">
         <f xml:space="preserve"> CONCATENATE(CEILING(Table1[[#This Row],[Current Part/Page]]/Table1[[#This Row],[Part/Page count]], 0.0001) * 100,"%")</f>
         <v>0%</v>
       </c>
-      <c r="F7" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H7" s="3" t="s">
-        <v>20</v>
+      <c r="F7" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J7" s="3"/>
     </row>
     <row r="8" spans="1:10" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
+      <c r="A8" s="12">
         <v>6</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>8</v>
+      <c r="B8" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="C8" s="1">
-        <v>500</v>
+        <v>504</v>
       </c>
       <c r="E8" s="5" t="str">
         <f xml:space="preserve"> CONCATENATE(CEILING(Table1[[#This Row],[Current Part/Page]]/Table1[[#This Row],[Part/Page count]], 0.0001) * 100,"%")</f>
         <v>0%</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J8" s="3"/>
     </row>
     <row r="9" spans="1:10" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
+      <c r="A9" s="12">
         <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="C9" s="1">
-        <v>3</v>
+        <v>500</v>
+      </c>
+      <c r="D9" s="1">
+        <v>15</v>
       </c>
       <c r="E9" s="5" t="str">
         <f xml:space="preserve"> CONCATENATE(CEILING(Table1[[#This Row],[Current Part/Page]]/Table1[[#This Row],[Part/Page count]], 0.0001) * 100,"%")</f>
-        <v>0%</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>20</v>
-      </c>
+        <v>3%</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J9" s="3"/>
     </row>
     <row r="10" spans="1:10" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
+      <c r="A10" s="12">
         <v>8</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C10" s="1">
         <v>3</v>
@@ -790,34 +886,37 @@
         <f xml:space="preserve"> CONCATENATE(CEILING(Table1[[#This Row],[Current Part/Page]]/Table1[[#This Row],[Part/Page count]], 0.0001) * 100,"%")</f>
         <v>0%</v>
       </c>
-      <c r="G10" s="1" t="s">
-        <v>20</v>
+      <c r="F10" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:10" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
+      <c r="A11" s="12">
         <v>9</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C11" s="1">
         <v>3</v>
       </c>
+      <c r="D11" s="1">
+        <v>1</v>
+      </c>
       <c r="E11" s="5" t="str">
         <f xml:space="preserve"> CONCATENATE(CEILING(Table1[[#This Row],[Current Part/Page]]/Table1[[#This Row],[Part/Page count]], 0.0001) * 100,"%")</f>
-        <v>0%</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>20</v>
+        <v>33.34%</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:10" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
+      <c r="A12" s="12">
         <v>10</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C12" s="1">
         <v>3</v>
@@ -826,105 +925,96 @@
         <f xml:space="preserve"> CONCATENATE(CEILING(Table1[[#This Row],[Current Part/Page]]/Table1[[#This Row],[Part/Page count]], 0.0001) * 100,"%")</f>
         <v>0%</v>
       </c>
-      <c r="I12" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
+      <c r="H12" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="12">
         <v>11</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="C13" s="1">
-        <v>400</v>
-      </c>
-      <c r="D13" s="1">
-        <v>20</v>
+        <v>3</v>
       </c>
       <c r="E13" s="5" t="str">
         <f xml:space="preserve"> CONCATENATE(CEILING(Table1[[#This Row],[Current Part/Page]]/Table1[[#This Row],[Part/Page count]], 0.0001) * 100,"%")</f>
-        <v>5%</v>
-      </c>
-      <c r="F13" s="1" t="s">
+        <v>0%</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="12">
+        <v>12</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" s="1">
+        <v>400</v>
+      </c>
+      <c r="D14" s="1">
         <v>20</v>
       </c>
-      <c r="G13" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="I13" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="J13" s="1"/>
-    </row>
-    <row r="14" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
-        <v>12</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C14" s="1">
-        <v>54</v>
-      </c>
-      <c r="D14" s="1"/>
       <c r="E14" s="5" t="str">
         <f xml:space="preserve"> CONCATENATE(CEILING(Table1[[#This Row],[Current Part/Page]]/Table1[[#This Row],[Part/Page count]], 0.0001) * 100,"%")</f>
-        <v>0%</v>
+        <v>5%</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="H14" s="1"/>
-      <c r="I14" s="1"/>
+        <v>19</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="J14" s="1"/>
     </row>
     <row r="15" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="1">
+      <c r="A15" s="12">
         <v>13</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="C15" s="1">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="D15" s="1"/>
       <c r="E15" s="5" t="str">
         <f xml:space="preserve"> CONCATENATE(CEILING(Table1[[#This Row],[Current Part/Page]]/Table1[[#This Row],[Part/Page count]], 0.0001) * 100,"%")</f>
         <v>0%</v>
       </c>
-      <c r="F15" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G15" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H15" s="3"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
     </row>
     <row r="16" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="1">
+      <c r="A16" s="12">
         <v>14</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="C16" s="1">
-        <v>100</v>
-      </c>
-      <c r="D16" s="1"/>
+        <v>60</v>
+      </c>
+      <c r="D16" s="1">
+        <v>1</v>
+      </c>
       <c r="E16" s="5" t="str">
         <f xml:space="preserve"> CONCATENATE(CEILING(Table1[[#This Row],[Current Part/Page]]/Table1[[#This Row],[Part/Page count]], 0.0001) * 100,"%")</f>
-        <v>0%</v>
+        <v>1.67%</v>
       </c>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
@@ -933,14 +1023,14 @@
       <c r="J16" s="1"/>
     </row>
     <row r="17" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="1">
+      <c r="A17" s="12">
         <v>15</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>13</v>
+        <v>30</v>
       </c>
       <c r="C17" s="1">
-        <v>100</v>
+        <v>60</v>
       </c>
       <c r="D17" s="1"/>
       <c r="E17" s="5" t="str">
@@ -954,29 +1044,121 @@
       <c r="J17" s="1"/>
     </row>
     <row r="18" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="1">
+      <c r="A18" s="12">
         <v>16</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="C18" s="1">
-        <v>236</v>
+        <v>60</v>
       </c>
       <c r="D18" s="1"/>
       <c r="E18" s="5" t="str">
         <f xml:space="preserve"> CONCATENATE(CEILING(Table1[[#This Row],[Current Part/Page]]/Table1[[#This Row],[Part/Page count]], 0.0001) * 100,"%")</f>
         <v>0%</v>
       </c>
-      <c r="F18" s="1"/>
-      <c r="G18" s="1"/>
+      <c r="F18" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
     </row>
-    <row r="19" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="20" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="21" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="19" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="12">
+        <v>17</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C19" s="1">
+        <v>50</v>
+      </c>
+      <c r="D19" s="1"/>
+      <c r="E19" s="5" t="str">
+        <f xml:space="preserve"> CONCATENATE(CEILING(Table1[[#This Row],[Current Part/Page]]/Table1[[#This Row],[Part/Page count]], 0.0001) * 100,"%")</f>
+        <v>0%</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H19" s="3"/>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1"/>
+    </row>
+    <row r="20" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="12">
+        <v>18</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C20" s="1">
+        <v>100</v>
+      </c>
+      <c r="D20" s="1"/>
+      <c r="E20" s="5" t="str">
+        <f xml:space="preserve"> CONCATENATE(CEILING(Table1[[#This Row],[Current Part/Page]]/Table1[[#This Row],[Part/Page count]], 0.0001) * 100,"%")</f>
+        <v>0%</v>
+      </c>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+      <c r="J20" s="1"/>
+    </row>
+    <row r="21" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="12">
+        <v>19</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C21" s="1">
+        <v>100</v>
+      </c>
+      <c r="D21" s="1"/>
+      <c r="E21" s="5" t="str">
+        <f xml:space="preserve"> CONCATENATE(CEILING(Table1[[#This Row],[Current Part/Page]]/Table1[[#This Row],[Part/Page count]], 0.0001) * 100,"%")</f>
+        <v>0%</v>
+      </c>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
+      <c r="J21" s="1"/>
+    </row>
+    <row r="22" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="12">
+        <v>20</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C22" s="1">
+        <v>236</v>
+      </c>
+      <c r="D22" s="1"/>
+      <c r="E22" s="5" t="str">
+        <f xml:space="preserve"> CONCATENATE(CEILING(Table1[[#This Row],[Current Part/Page]]/Table1[[#This Row],[Part/Page count]], 0.0001) * 100,"%")</f>
+        <v>0%</v>
+      </c>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
+      <c r="J22" s="1"/>
+    </row>
+    <row r="23" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="F1:I1"/>
@@ -987,4 +1169,795 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J56"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="7.7109375" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" customWidth="1"/>
+    <col min="4" max="4" width="11" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" customWidth="1"/>
+    <col min="6" max="6" width="16.28515625" customWidth="1"/>
+    <col min="8" max="8" width="9.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" s="6" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="H1" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
+    </row>
+    <row r="2" spans="1:10" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="10">
+        <v>20</v>
+      </c>
+      <c r="C2" s="10">
+        <v>21</v>
+      </c>
+      <c r="D2" s="10">
+        <v>20</v>
+      </c>
+      <c r="E2" s="10">
+        <v>20</v>
+      </c>
+      <c r="F2" s="10">
+        <f xml:space="preserve"> SUM(B2, C2, D2, E2)</f>
+        <v>81</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="10"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10">
+        <f t="shared" ref="F3:F55" si="0" xml:space="preserve"> SUM(B3, C3, D3, E3)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="10"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="10"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="10"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="10"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" s="10"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9" s="10"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
+      <c r="B10" s="10"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>10</v>
+      </c>
+      <c r="B11" s="10"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>11</v>
+      </c>
+      <c r="B12" s="10"/>
+      <c r="C12" s="10"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>12</v>
+      </c>
+      <c r="B13" s="10"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>13</v>
+      </c>
+      <c r="B14" s="10"/>
+      <c r="C14" s="10"/>
+      <c r="D14" s="10"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>14</v>
+      </c>
+      <c r="B15" s="10"/>
+      <c r="C15" s="10"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>15</v>
+      </c>
+      <c r="B16" s="10"/>
+      <c r="C16" s="10"/>
+      <c r="D16" s="10"/>
+      <c r="E16" s="10"/>
+      <c r="F16" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>16</v>
+      </c>
+      <c r="B17" s="10"/>
+      <c r="C17" s="10"/>
+      <c r="D17" s="10"/>
+      <c r="E17" s="10"/>
+      <c r="F17" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>17</v>
+      </c>
+      <c r="B18" s="10"/>
+      <c r="C18" s="10"/>
+      <c r="D18" s="10"/>
+      <c r="E18" s="10"/>
+      <c r="F18" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>18</v>
+      </c>
+      <c r="B19" s="10"/>
+      <c r="C19" s="10"/>
+      <c r="D19" s="10"/>
+      <c r="E19" s="10"/>
+      <c r="F19" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>19</v>
+      </c>
+      <c r="B20" s="10"/>
+      <c r="C20" s="10"/>
+      <c r="D20" s="10"/>
+      <c r="E20" s="10"/>
+      <c r="F20" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>20</v>
+      </c>
+      <c r="B21" s="10"/>
+      <c r="C21" s="10"/>
+      <c r="D21" s="10"/>
+      <c r="E21" s="10"/>
+      <c r="F21" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>21</v>
+      </c>
+      <c r="B22" s="10"/>
+      <c r="C22" s="10"/>
+      <c r="D22" s="10"/>
+      <c r="E22" s="10"/>
+      <c r="F22" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>22</v>
+      </c>
+      <c r="B23" s="10"/>
+      <c r="C23" s="10"/>
+      <c r="D23" s="10"/>
+      <c r="E23" s="10"/>
+      <c r="F23" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>23</v>
+      </c>
+      <c r="B24" s="10"/>
+      <c r="C24" s="10"/>
+      <c r="D24" s="10"/>
+      <c r="E24" s="10"/>
+      <c r="F24" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <v>24</v>
+      </c>
+      <c r="B25" s="10"/>
+      <c r="C25" s="10"/>
+      <c r="D25" s="10"/>
+      <c r="E25" s="10"/>
+      <c r="F25" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
+        <v>25</v>
+      </c>
+      <c r="B26" s="10"/>
+      <c r="C26" s="10"/>
+      <c r="D26" s="10"/>
+      <c r="E26" s="10"/>
+      <c r="F26" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
+        <v>26</v>
+      </c>
+      <c r="B27" s="10"/>
+      <c r="C27" s="10"/>
+      <c r="D27" s="10"/>
+      <c r="E27" s="10"/>
+      <c r="F27" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
+        <v>27</v>
+      </c>
+      <c r="B28" s="10"/>
+      <c r="C28" s="10"/>
+      <c r="D28" s="10"/>
+      <c r="E28" s="10"/>
+      <c r="F28" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
+        <v>28</v>
+      </c>
+      <c r="B29" s="10"/>
+      <c r="C29" s="10"/>
+      <c r="D29" s="10"/>
+      <c r="E29" s="10"/>
+      <c r="F29" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
+        <v>29</v>
+      </c>
+      <c r="B30" s="10"/>
+      <c r="C30" s="10"/>
+      <c r="D30" s="10"/>
+      <c r="E30" s="10"/>
+      <c r="F30" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
+        <v>30</v>
+      </c>
+      <c r="B31" s="10"/>
+      <c r="C31" s="10"/>
+      <c r="D31" s="10"/>
+      <c r="E31" s="10"/>
+      <c r="F31" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="1">
+        <v>31</v>
+      </c>
+      <c r="B32" s="10"/>
+      <c r="C32" s="10"/>
+      <c r="D32" s="10"/>
+      <c r="E32" s="10"/>
+      <c r="F32" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="1">
+        <v>32</v>
+      </c>
+      <c r="B33" s="10"/>
+      <c r="C33" s="10"/>
+      <c r="D33" s="10"/>
+      <c r="E33" s="10"/>
+      <c r="F33" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="1">
+        <v>33</v>
+      </c>
+      <c r="B34" s="10"/>
+      <c r="C34" s="10"/>
+      <c r="D34" s="10"/>
+      <c r="E34" s="10"/>
+      <c r="F34" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="1">
+        <v>34</v>
+      </c>
+      <c r="B35" s="10"/>
+      <c r="C35" s="10"/>
+      <c r="D35" s="10"/>
+      <c r="E35" s="10"/>
+      <c r="F35" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="1">
+        <v>35</v>
+      </c>
+      <c r="B36" s="10"/>
+      <c r="C36" s="10"/>
+      <c r="D36" s="10"/>
+      <c r="E36" s="10"/>
+      <c r="F36" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="1">
+        <v>36</v>
+      </c>
+      <c r="B37" s="10"/>
+      <c r="C37" s="10"/>
+      <c r="D37" s="10"/>
+      <c r="E37" s="10"/>
+      <c r="F37" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="1">
+        <v>37</v>
+      </c>
+      <c r="B38" s="10"/>
+      <c r="C38" s="10"/>
+      <c r="D38" s="10"/>
+      <c r="E38" s="10"/>
+      <c r="F38" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="1">
+        <v>38</v>
+      </c>
+      <c r="B39" s="10"/>
+      <c r="C39" s="10"/>
+      <c r="D39" s="10"/>
+      <c r="E39" s="10"/>
+      <c r="F39" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="1">
+        <v>39</v>
+      </c>
+      <c r="B40" s="10"/>
+      <c r="C40" s="10"/>
+      <c r="D40" s="10"/>
+      <c r="E40" s="10"/>
+      <c r="F40" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="1">
+        <v>40</v>
+      </c>
+      <c r="B41" s="10"/>
+      <c r="C41" s="10"/>
+      <c r="D41" s="10"/>
+      <c r="E41" s="10"/>
+      <c r="F41" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="1">
+        <v>41</v>
+      </c>
+      <c r="B42" s="10"/>
+      <c r="C42" s="10"/>
+      <c r="D42" s="10"/>
+      <c r="E42" s="10"/>
+      <c r="F42" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="1">
+        <v>42</v>
+      </c>
+      <c r="B43" s="10"/>
+      <c r="C43" s="10"/>
+      <c r="D43" s="10"/>
+      <c r="E43" s="10"/>
+      <c r="F43" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="1">
+        <v>43</v>
+      </c>
+      <c r="B44" s="10"/>
+      <c r="C44" s="10"/>
+      <c r="D44" s="10"/>
+      <c r="E44" s="10"/>
+      <c r="F44" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="1">
+        <v>44</v>
+      </c>
+      <c r="B45" s="10"/>
+      <c r="C45" s="10"/>
+      <c r="D45" s="10"/>
+      <c r="E45" s="10"/>
+      <c r="F45" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="1">
+        <v>45</v>
+      </c>
+      <c r="B46" s="10"/>
+      <c r="C46" s="10"/>
+      <c r="D46" s="10"/>
+      <c r="E46" s="10"/>
+      <c r="F46" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="1">
+        <v>46</v>
+      </c>
+      <c r="B47" s="10"/>
+      <c r="C47" s="10"/>
+      <c r="D47" s="10"/>
+      <c r="E47" s="10"/>
+      <c r="F47" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="1">
+        <v>47</v>
+      </c>
+      <c r="B48" s="10"/>
+      <c r="C48" s="10"/>
+      <c r="D48" s="10"/>
+      <c r="E48" s="10"/>
+      <c r="F48" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="1">
+        <v>48</v>
+      </c>
+      <c r="B49" s="10"/>
+      <c r="C49" s="10"/>
+      <c r="D49" s="10"/>
+      <c r="E49" s="10"/>
+      <c r="F49" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="1">
+        <v>49</v>
+      </c>
+      <c r="B50" s="10"/>
+      <c r="C50" s="10"/>
+      <c r="D50" s="10"/>
+      <c r="E50" s="10"/>
+      <c r="F50" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="1">
+        <v>50</v>
+      </c>
+      <c r="B51" s="10"/>
+      <c r="C51" s="10"/>
+      <c r="D51" s="10"/>
+      <c r="E51" s="10"/>
+      <c r="F51" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="1">
+        <v>51</v>
+      </c>
+      <c r="B52" s="10"/>
+      <c r="C52" s="10"/>
+      <c r="D52" s="10"/>
+      <c r="E52" s="10"/>
+      <c r="F52" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="1">
+        <v>52</v>
+      </c>
+      <c r="B53" s="10"/>
+      <c r="C53" s="10"/>
+      <c r="D53" s="10"/>
+      <c r="E53" s="10"/>
+      <c r="F53" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="1">
+        <v>53</v>
+      </c>
+      <c r="B54" s="10"/>
+      <c r="C54" s="10"/>
+      <c r="D54" s="10"/>
+      <c r="E54" s="10"/>
+      <c r="F54" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="1">
+        <v>54</v>
+      </c>
+      <c r="B55" s="10"/>
+      <c r="C55" s="10"/>
+      <c r="D55" s="10"/>
+      <c r="E55" s="10"/>
+      <c r="F55" s="10">
+        <f xml:space="preserve"> SUM(B55, C55, D55, E55)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B56" s="10">
+        <f xml:space="preserve"> AVERAGE(B2:B55)</f>
+        <v>20</v>
+      </c>
+      <c r="C56" s="10">
+        <f t="shared" ref="C56:F56" si="1" xml:space="preserve"> AVERAGE(C2:C55)</f>
+        <v>21</v>
+      </c>
+      <c r="D56" s="10">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="E56" s="10">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="F56" s="10">
+        <f xml:space="preserve"> SUM(B56, C56, D56, E56)</f>
+        <v>81</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="H1:J1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" copies="0" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update my progress and some other resources to read
</commit_message>
<xml_diff>
--- a/TOEFL/Progress.xlsx
+++ b/TOEFL/Progress.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="5850" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="7020" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Progree" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="40">
   <si>
     <t>Book/CD Name</t>
   </si>
@@ -55,12 +55,6 @@
     <t>TED Talks</t>
   </si>
   <si>
-    <t>Skills for the TOEFL iBT test Book</t>
-  </si>
-  <si>
-    <t>Skills for the TOEFL iBT test CD</t>
-  </si>
-  <si>
     <t>Oxford English Grammar Course Teachers' Tests</t>
   </si>
   <si>
@@ -88,9 +82,6 @@
     <t>Tasks they are related to.</t>
   </si>
   <si>
-    <t>Needs to be repeated</t>
-  </si>
-  <si>
     <t>Baron's Wriring for the TOEFL iBT</t>
   </si>
   <si>
@@ -128,6 +119,27 @@
   </si>
   <si>
     <t>Oxford English Grammar Course Book Tests</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.5, 2.7, </t>
+  </si>
+  <si>
+    <t>TOEFL Grammar Tests Book</t>
+  </si>
+  <si>
+    <t>Skills for the TOEFL iBT test Reading &amp; Writing CD</t>
+  </si>
+  <si>
+    <t>Skills for the TOEFL iBT test Reading &amp; Writing Book</t>
+  </si>
+  <si>
+    <t>Needs to be reviewed</t>
+  </si>
+  <si>
+    <t>17, 28, 29</t>
+  </si>
+  <si>
+    <t>Review Words Flash Cards</t>
   </si>
 </sst>
 </file>
@@ -215,17 +227,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -235,6 +238,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -332,8 +344,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A2:J22" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18">
-  <autoFilter ref="A2:J22"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A2:J24" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18">
+  <autoFilter ref="A2:J24"/>
   <tableColumns count="10">
     <tableColumn id="1" name="No." dataDxfId="17"/>
     <tableColumn id="2" name="Book/CD Name" dataDxfId="16"/>
@@ -346,7 +358,7 @@
     <tableColumn id="10" name="Listening" dataDxfId="11"/>
     <tableColumn id="9" name="Speaking" dataDxfId="10"/>
     <tableColumn id="8" name="Writing" dataDxfId="9"/>
-    <tableColumn id="12" name="Needs to be repeated" dataDxfId="8"/>
+    <tableColumn id="12" name="Needs to be reviewed" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -634,13 +646,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="45.140625" customWidth="1"/>
+    <col min="1" max="1" width="7.5703125" customWidth="1"/>
+    <col min="2" max="2" width="46.28515625" customWidth="1"/>
     <col min="3" max="3" width="10.42578125" customWidth="1"/>
     <col min="4" max="4" width="11" customWidth="1"/>
     <col min="5" max="5" width="15" style="4" customWidth="1"/>
@@ -652,12 +665,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F1" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
+      <c r="F1" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
     </row>
     <row r="2" spans="1:10" s="6" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
@@ -676,19 +689,19 @@
         <v>4</v>
       </c>
       <c r="F2" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="I2" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="G2" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="H2" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="I2" s="6" t="s">
-        <v>18</v>
-      </c>
       <c r="J2" s="6" t="s">
-        <v>22</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:10" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -702,26 +715,26 @@
         <v>17</v>
       </c>
       <c r="D3" s="1">
-        <v>2.1</v>
+        <v>3.1</v>
       </c>
       <c r="E3" s="5" t="str">
         <f xml:space="preserve"> CONCATENATE(CEILING(Table1[[#This Row],[Current Part/Page]]/Table1[[#This Row],[Part/Page count]], 0.0001) * 100,"%")</f>
-        <v>12.36%</v>
+        <v>18.24%</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="J3" s="3">
-        <v>1.5</v>
+        <v>17</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:10" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -735,29 +748,31 @@
         <v>310</v>
       </c>
       <c r="D4" s="1">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="E4" s="5" t="str">
         <f xml:space="preserve"> CONCATENATE(CEILING(Table1[[#This Row],[Current Part/Page]]/Table1[[#This Row],[Part/Page count]], 0.0001) * 100,"%")</f>
-        <v>5.17%</v>
+        <v>9.68%</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="J4" s="3"/>
+        <v>18</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="5" spans="1:10" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C5" s="1">
         <v>22</v>
@@ -767,36 +782,36 @@
         <v>0%</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="J5" s="3"/>
     </row>
-    <row r="6" spans="1:10" s="12" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="12">
+    <row r="6" spans="1:10" s="9" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="9">
         <v>4</v>
       </c>
-      <c r="B6" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="C6" s="12">
-        <v>17</v>
-      </c>
-      <c r="E6" s="14" t="str">
+      <c r="B6" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" s="9">
+        <v>17</v>
+      </c>
+      <c r="E6" s="11" t="str">
         <f xml:space="preserve"> CONCATENATE(CEILING(Table1[[#This Row],[Current Part/Page]]/Table1[[#This Row],[Part/Page count]], 0.0001) * 100,"%")</f>
         <v>0%</v>
       </c>
-      <c r="I6" s="13"/>
-      <c r="J6" s="13"/>
+      <c r="I6" s="10"/>
+      <c r="J6" s="10"/>
     </row>
     <row r="7" spans="1:10" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="12">
+      <c r="A7" s="9">
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C7" s="1">
         <v>17</v>
@@ -806,15 +821,15 @@
         <v>0%</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="J7" s="3"/>
     </row>
     <row r="8" spans="1:10" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="12">
+      <c r="A8" s="9">
         <v>6</v>
       </c>
       <c r="B8" s="2" t="s">
@@ -828,21 +843,21 @@
         <v>0%</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="J8" s="3"/>
     </row>
     <row r="9" spans="1:10" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="12">
+      <c r="A9" s="9">
         <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -852,89 +867,100 @@
         <v>500</v>
       </c>
       <c r="D9" s="1">
-        <v>15</v>
+        <v>45</v>
       </c>
       <c r="E9" s="5" t="str">
         <f xml:space="preserve"> CONCATENATE(CEILING(Table1[[#This Row],[Current Part/Page]]/Table1[[#This Row],[Part/Page count]], 0.0001) * 100,"%")</f>
-        <v>3%</v>
+        <v>9%</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="J9" s="3"/>
     </row>
     <row r="10" spans="1:10" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="12">
+      <c r="A10" s="9">
         <v>8</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C10" s="1">
-        <v>3</v>
-      </c>
-      <c r="E10" s="5" t="str">
+      <c r="B10" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C10" s="9">
+        <v>500</v>
+      </c>
+      <c r="D10" s="9"/>
+      <c r="E10" s="11" t="str">
         <f xml:space="preserve"> CONCATENATE(CEILING(Table1[[#This Row],[Current Part/Page]]/Table1[[#This Row],[Part/Page count]], 0.0001) * 100,"%")</f>
         <v>0%</v>
       </c>
-      <c r="F10" s="1" t="s">
-        <v>19</v>
-      </c>
+      <c r="F10" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="G10" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="H10" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="I10" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="J10" s="10"/>
     </row>
     <row r="11" spans="1:10" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="12">
+      <c r="A11" s="9">
         <v>9</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C11" s="1">
         <v>3</v>
       </c>
-      <c r="D11" s="1">
-        <v>1</v>
-      </c>
       <c r="E11" s="5" t="str">
         <f xml:space="preserve"> CONCATENATE(CEILING(Table1[[#This Row],[Current Part/Page]]/Table1[[#This Row],[Part/Page count]], 0.0001) * 100,"%")</f>
-        <v>33.34%</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>19</v>
+        <v>0%</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:10" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="12">
+      <c r="A12" s="9">
         <v>10</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C12" s="1">
         <v>3</v>
       </c>
+      <c r="D12" s="1">
+        <v>1</v>
+      </c>
       <c r="E12" s="5" t="str">
         <f xml:space="preserve"> CONCATENATE(CEILING(Table1[[#This Row],[Current Part/Page]]/Table1[[#This Row],[Part/Page count]], 0.0001) * 100,"%")</f>
-        <v>0%</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>19</v>
+        <v>33.34%</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:10" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="12">
+      <c r="A13" s="9">
         <v>11</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C13" s="1">
         <v>3</v>
@@ -943,78 +969,78 @@
         <f xml:space="preserve"> CONCATENATE(CEILING(Table1[[#This Row],[Current Part/Page]]/Table1[[#This Row],[Part/Page count]], 0.0001) * 100,"%")</f>
         <v>0%</v>
       </c>
-      <c r="I13" s="1" t="s">
-        <v>19</v>
+      <c r="H13" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="12">
+      <c r="A14" s="9">
         <v>12</v>
       </c>
       <c r="B14" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" s="1">
+        <v>3</v>
+      </c>
+      <c r="D14" s="1"/>
+      <c r="E14" s="5" t="str">
+        <f xml:space="preserve"> CONCATENATE(CEILING(Table1[[#This Row],[Current Part/Page]]/Table1[[#This Row],[Part/Page count]], 0.0001) * 100,"%")</f>
+        <v>0%</v>
+      </c>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J14" s="1"/>
+    </row>
+    <row r="15" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="9">
+        <v>13</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C14" s="1">
+      <c r="C15" s="1">
         <v>400</v>
       </c>
-      <c r="D14" s="1">
+      <c r="D15" s="1">
         <v>20</v>
       </c>
-      <c r="E14" s="5" t="str">
+      <c r="E15" s="5" t="str">
         <f xml:space="preserve"> CONCATENATE(CEILING(Table1[[#This Row],[Current Part/Page]]/Table1[[#This Row],[Part/Page count]], 0.0001) * 100,"%")</f>
         <v>5%</v>
       </c>
-      <c r="F14" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="H14" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="I14" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="J14" s="1"/>
-    </row>
-    <row r="15" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="12">
-        <v>13</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C15" s="1">
-        <v>60</v>
-      </c>
-      <c r="D15" s="1"/>
-      <c r="E15" s="5" t="str">
-        <f xml:space="preserve"> CONCATENATE(CEILING(Table1[[#This Row],[Current Part/Page]]/Table1[[#This Row],[Part/Page count]], 0.0001) * 100,"%")</f>
-        <v>0%</v>
-      </c>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
-      <c r="I15" s="1"/>
+      <c r="F15" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="J15" s="1"/>
     </row>
     <row r="16" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="12">
+      <c r="A16" s="9">
         <v>14</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C16" s="1">
         <v>60</v>
       </c>
-      <c r="D16" s="1">
-        <v>1</v>
-      </c>
+      <c r="D16" s="1"/>
       <c r="E16" s="5" t="str">
         <f xml:space="preserve"> CONCATENATE(CEILING(Table1[[#This Row],[Current Part/Page]]/Table1[[#This Row],[Part/Page count]], 0.0001) * 100,"%")</f>
-        <v>1.67%</v>
+        <v>0%</v>
       </c>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
@@ -1023,19 +1049,21 @@
       <c r="J16" s="1"/>
     </row>
     <row r="17" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="12">
+      <c r="A17" s="9">
         <v>15</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C17" s="1">
         <v>60</v>
       </c>
-      <c r="D17" s="1"/>
+      <c r="D17" s="1">
+        <v>2</v>
+      </c>
       <c r="E17" s="5" t="str">
         <f xml:space="preserve"> CONCATENATE(CEILING(Table1[[#This Row],[Current Part/Page]]/Table1[[#This Row],[Part/Page count]], 0.0001) * 100,"%")</f>
-        <v>0%</v>
+        <v>3.34%</v>
       </c>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
@@ -1044,11 +1072,11 @@
       <c r="J17" s="1"/>
     </row>
     <row r="18" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="12">
+      <c r="A18" s="9">
         <v>16</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C18" s="1">
         <v>60</v>
@@ -1058,25 +1086,21 @@
         <f xml:space="preserve"> CONCATENATE(CEILING(Table1[[#This Row],[Current Part/Page]]/Table1[[#This Row],[Part/Page count]], 0.0001) * 100,"%")</f>
         <v>0%</v>
       </c>
-      <c r="F18" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>19</v>
-      </c>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
     </row>
     <row r="19" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="12">
+      <c r="A19" s="9">
         <v>17</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="C19" s="1">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="D19" s="1"/>
       <c r="E19" s="5" t="str">
@@ -1084,80 +1108,132 @@
         <v>0%</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G19" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="H19" s="3"/>
+        <v>17</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H19" s="1"/>
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
     </row>
     <row r="20" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="12">
+      <c r="A20" s="9">
         <v>18</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C20" s="1">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="D20" s="1"/>
       <c r="E20" s="5" t="str">
         <f xml:space="preserve"> CONCATENATE(CEILING(Table1[[#This Row],[Current Part/Page]]/Table1[[#This Row],[Part/Page count]], 0.0001) * 100,"%")</f>
         <v>0%</v>
       </c>
-      <c r="F20" s="1"/>
-      <c r="G20" s="1"/>
-      <c r="H20" s="1"/>
+      <c r="F20" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H20" s="3"/>
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
     </row>
     <row r="21" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="12">
+      <c r="A21" s="9">
         <v>19</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>12</v>
+        <v>36</v>
       </c>
       <c r="C21" s="1">
-        <v>100</v>
+        <v>170</v>
       </c>
       <c r="D21" s="1"/>
       <c r="E21" s="5" t="str">
         <f xml:space="preserve"> CONCATENATE(CEILING(Table1[[#This Row],[Current Part/Page]]/Table1[[#This Row],[Part/Page count]], 0.0001) * 100,"%")</f>
         <v>0%</v>
       </c>
-      <c r="F21" s="1"/>
+      <c r="F21" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
-      <c r="I21" s="1"/>
+      <c r="I21" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="J21" s="1"/>
     </row>
     <row r="22" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="12">
+      <c r="A22" s="9">
         <v>20</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="C22" s="1">
-        <v>236</v>
+        <v>100</v>
       </c>
       <c r="D22" s="1"/>
       <c r="E22" s="5" t="str">
         <f xml:space="preserve"> CONCATENATE(CEILING(Table1[[#This Row],[Current Part/Page]]/Table1[[#This Row],[Part/Page count]], 0.0001) * 100,"%")</f>
         <v>0%</v>
       </c>
-      <c r="F22" s="1"/>
+      <c r="F22" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
-      <c r="I22" s="1"/>
+      <c r="I22" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="J22" s="1"/>
     </row>
-    <row r="23" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="9">
+        <v>21</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C23" s="1">
+        <v>236</v>
+      </c>
+      <c r="D23" s="1"/>
+      <c r="E23" s="5" t="str">
+        <f xml:space="preserve"> CONCATENATE(CEILING(Table1[[#This Row],[Current Part/Page]]/Table1[[#This Row],[Part/Page count]], 0.0001) * 100,"%")</f>
+        <v>0%</v>
+      </c>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1"/>
+      <c r="J23" s="1"/>
+    </row>
+    <row r="24" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="9">
+        <v>22</v>
+      </c>
+      <c r="B24" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="C24" s="9">
+        <v>200</v>
+      </c>
+      <c r="D24" s="9"/>
+      <c r="E24" s="11" t="str">
+        <f xml:space="preserve"> CONCATENATE(CEILING(Table1[[#This Row],[Current Part/Page]]/Table1[[#This Row],[Part/Page count]], 0.0001) * 100,"%")</f>
+        <v>0%</v>
+      </c>
+      <c r="F24" s="9"/>
+      <c r="G24" s="9"/>
+      <c r="H24" s="9"/>
+      <c r="I24" s="9"/>
+      <c r="J24" s="9"/>
+    </row>
     <row r="25" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="1">
@@ -1176,7 +1252,7 @@
   <dimension ref="A1:J56"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1195,43 +1271,43 @@
         <v>1</v>
       </c>
       <c r="B1" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>18</v>
-      </c>
       <c r="F1" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="H1" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="I1" s="11"/>
-      <c r="J1" s="11"/>
+        <v>30</v>
+      </c>
+      <c r="H1" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
     </row>
     <row r="2" spans="1:10" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2" s="10">
+      <c r="B2" s="8">
         <v>20</v>
       </c>
-      <c r="C2" s="10">
+      <c r="C2" s="8">
         <v>21</v>
       </c>
-      <c r="D2" s="10">
+      <c r="D2" s="8">
         <v>20</v>
       </c>
-      <c r="E2" s="10">
+      <c r="E2" s="8">
         <v>20</v>
       </c>
-      <c r="F2" s="10">
+      <c r="F2" s="8">
         <f xml:space="preserve"> SUM(B2, C2, D2, E2)</f>
         <v>81</v>
       </c>
@@ -1240,24 +1316,26 @@
       <c r="A3" s="1">
         <v>2</v>
       </c>
-      <c r="B3" s="10"/>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="10">
-        <f t="shared" ref="F3:F55" si="0" xml:space="preserve"> SUM(B3, C3, D3, E3)</f>
-        <v>0</v>
+      <c r="B3" s="8"/>
+      <c r="C3" s="8">
+        <v>25</v>
+      </c>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8">
+        <f t="shared" ref="F3:F54" si="0" xml:space="preserve"> SUM(B3, C3, D3, E3)</f>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:10" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
-      <c r="B4" s="10"/>
-      <c r="C4" s="10"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10"/>
-      <c r="F4" s="10">
+      <c r="B4" s="8"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1266,11 +1344,11 @@
       <c r="A5" s="1">
         <v>4</v>
       </c>
-      <c r="B5" s="10"/>
-      <c r="C5" s="10"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="10">
+      <c r="B5" s="8"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1279,11 +1357,11 @@
       <c r="A6" s="1">
         <v>5</v>
       </c>
-      <c r="B6" s="10"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10">
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1292,11 +1370,11 @@
       <c r="A7" s="1">
         <v>6</v>
       </c>
-      <c r="B7" s="10"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="10">
+      <c r="B7" s="8"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1305,11 +1383,11 @@
       <c r="A8" s="1">
         <v>7</v>
       </c>
-      <c r="B8" s="10"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="10">
+      <c r="B8" s="8"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1318,11 +1396,11 @@
       <c r="A9" s="1">
         <v>8</v>
       </c>
-      <c r="B9" s="10"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="10">
+      <c r="B9" s="8"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1331,11 +1409,11 @@
       <c r="A10" s="1">
         <v>9</v>
       </c>
-      <c r="B10" s="10"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="10">
+      <c r="B10" s="8"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1344,11 +1422,11 @@
       <c r="A11" s="1">
         <v>10</v>
       </c>
-      <c r="B11" s="10"/>
-      <c r="C11" s="10"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="10"/>
-      <c r="F11" s="10">
+      <c r="B11" s="8"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1357,11 +1435,11 @@
       <c r="A12" s="1">
         <v>11</v>
       </c>
-      <c r="B12" s="10"/>
-      <c r="C12" s="10"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="10"/>
-      <c r="F12" s="10">
+      <c r="B12" s="8"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1370,11 +1448,11 @@
       <c r="A13" s="1">
         <v>12</v>
       </c>
-      <c r="B13" s="10"/>
-      <c r="C13" s="10"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="10"/>
-      <c r="F13" s="10">
+      <c r="B13" s="8"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1383,11 +1461,11 @@
       <c r="A14" s="1">
         <v>13</v>
       </c>
-      <c r="B14" s="10"/>
-      <c r="C14" s="10"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="10"/>
-      <c r="F14" s="10">
+      <c r="B14" s="8"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1396,11 +1474,11 @@
       <c r="A15" s="1">
         <v>14</v>
       </c>
-      <c r="B15" s="10"/>
-      <c r="C15" s="10"/>
-      <c r="D15" s="10"/>
-      <c r="E15" s="10"/>
-      <c r="F15" s="10">
+      <c r="B15" s="8"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1409,11 +1487,11 @@
       <c r="A16" s="1">
         <v>15</v>
       </c>
-      <c r="B16" s="10"/>
-      <c r="C16" s="10"/>
-      <c r="D16" s="10"/>
-      <c r="E16" s="10"/>
-      <c r="F16" s="10">
+      <c r="B16" s="8"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1422,11 +1500,11 @@
       <c r="A17" s="1">
         <v>16</v>
       </c>
-      <c r="B17" s="10"/>
-      <c r="C17" s="10"/>
-      <c r="D17" s="10"/>
-      <c r="E17" s="10"/>
-      <c r="F17" s="10">
+      <c r="B17" s="8"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1435,11 +1513,11 @@
       <c r="A18" s="1">
         <v>17</v>
       </c>
-      <c r="B18" s="10"/>
-      <c r="C18" s="10"/>
-      <c r="D18" s="10"/>
-      <c r="E18" s="10"/>
-      <c r="F18" s="10">
+      <c r="B18" s="8"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="8"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1448,11 +1526,11 @@
       <c r="A19" s="1">
         <v>18</v>
       </c>
-      <c r="B19" s="10"/>
-      <c r="C19" s="10"/>
-      <c r="D19" s="10"/>
-      <c r="E19" s="10"/>
-      <c r="F19" s="10">
+      <c r="B19" s="8"/>
+      <c r="C19" s="8"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1461,11 +1539,11 @@
       <c r="A20" s="1">
         <v>19</v>
       </c>
-      <c r="B20" s="10"/>
-      <c r="C20" s="10"/>
-      <c r="D20" s="10"/>
-      <c r="E20" s="10"/>
-      <c r="F20" s="10">
+      <c r="B20" s="8"/>
+      <c r="C20" s="8"/>
+      <c r="D20" s="8"/>
+      <c r="E20" s="8"/>
+      <c r="F20" s="8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1474,11 +1552,11 @@
       <c r="A21" s="1">
         <v>20</v>
       </c>
-      <c r="B21" s="10"/>
-      <c r="C21" s="10"/>
-      <c r="D21" s="10"/>
-      <c r="E21" s="10"/>
-      <c r="F21" s="10">
+      <c r="B21" s="8"/>
+      <c r="C21" s="8"/>
+      <c r="D21" s="8"/>
+      <c r="E21" s="8"/>
+      <c r="F21" s="8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1487,11 +1565,11 @@
       <c r="A22" s="1">
         <v>21</v>
       </c>
-      <c r="B22" s="10"/>
-      <c r="C22" s="10"/>
-      <c r="D22" s="10"/>
-      <c r="E22" s="10"/>
-      <c r="F22" s="10">
+      <c r="B22" s="8"/>
+      <c r="C22" s="8"/>
+      <c r="D22" s="8"/>
+      <c r="E22" s="8"/>
+      <c r="F22" s="8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1500,11 +1578,11 @@
       <c r="A23" s="1">
         <v>22</v>
       </c>
-      <c r="B23" s="10"/>
-      <c r="C23" s="10"/>
-      <c r="D23" s="10"/>
-      <c r="E23" s="10"/>
-      <c r="F23" s="10">
+      <c r="B23" s="8"/>
+      <c r="C23" s="8"/>
+      <c r="D23" s="8"/>
+      <c r="E23" s="8"/>
+      <c r="F23" s="8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1513,11 +1591,11 @@
       <c r="A24" s="1">
         <v>23</v>
       </c>
-      <c r="B24" s="10"/>
-      <c r="C24" s="10"/>
-      <c r="D24" s="10"/>
-      <c r="E24" s="10"/>
-      <c r="F24" s="10">
+      <c r="B24" s="8"/>
+      <c r="C24" s="8"/>
+      <c r="D24" s="8"/>
+      <c r="E24" s="8"/>
+      <c r="F24" s="8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1526,11 +1604,11 @@
       <c r="A25" s="1">
         <v>24</v>
       </c>
-      <c r="B25" s="10"/>
-      <c r="C25" s="10"/>
-      <c r="D25" s="10"/>
-      <c r="E25" s="10"/>
-      <c r="F25" s="10">
+      <c r="B25" s="8"/>
+      <c r="C25" s="8"/>
+      <c r="D25" s="8"/>
+      <c r="E25" s="8"/>
+      <c r="F25" s="8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1539,11 +1617,11 @@
       <c r="A26" s="1">
         <v>25</v>
       </c>
-      <c r="B26" s="10"/>
-      <c r="C26" s="10"/>
-      <c r="D26" s="10"/>
-      <c r="E26" s="10"/>
-      <c r="F26" s="10">
+      <c r="B26" s="8"/>
+      <c r="C26" s="8"/>
+      <c r="D26" s="8"/>
+      <c r="E26" s="8"/>
+      <c r="F26" s="8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1552,11 +1630,11 @@
       <c r="A27" s="1">
         <v>26</v>
       </c>
-      <c r="B27" s="10"/>
-      <c r="C27" s="10"/>
-      <c r="D27" s="10"/>
-      <c r="E27" s="10"/>
-      <c r="F27" s="10">
+      <c r="B27" s="8"/>
+      <c r="C27" s="8"/>
+      <c r="D27" s="8"/>
+      <c r="E27" s="8"/>
+      <c r="F27" s="8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1565,11 +1643,11 @@
       <c r="A28" s="1">
         <v>27</v>
       </c>
-      <c r="B28" s="10"/>
-      <c r="C28" s="10"/>
-      <c r="D28" s="10"/>
-      <c r="E28" s="10"/>
-      <c r="F28" s="10">
+      <c r="B28" s="8"/>
+      <c r="C28" s="8"/>
+      <c r="D28" s="8"/>
+      <c r="E28" s="8"/>
+      <c r="F28" s="8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1578,11 +1656,11 @@
       <c r="A29" s="1">
         <v>28</v>
       </c>
-      <c r="B29" s="10"/>
-      <c r="C29" s="10"/>
-      <c r="D29" s="10"/>
-      <c r="E29" s="10"/>
-      <c r="F29" s="10">
+      <c r="B29" s="8"/>
+      <c r="C29" s="8"/>
+      <c r="D29" s="8"/>
+      <c r="E29" s="8"/>
+      <c r="F29" s="8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1591,11 +1669,11 @@
       <c r="A30" s="1">
         <v>29</v>
       </c>
-      <c r="B30" s="10"/>
-      <c r="C30" s="10"/>
-      <c r="D30" s="10"/>
-      <c r="E30" s="10"/>
-      <c r="F30" s="10">
+      <c r="B30" s="8"/>
+      <c r="C30" s="8"/>
+      <c r="D30" s="8"/>
+      <c r="E30" s="8"/>
+      <c r="F30" s="8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1604,11 +1682,11 @@
       <c r="A31" s="1">
         <v>30</v>
       </c>
-      <c r="B31" s="10"/>
-      <c r="C31" s="10"/>
-      <c r="D31" s="10"/>
-      <c r="E31" s="10"/>
-      <c r="F31" s="10">
+      <c r="B31" s="8"/>
+      <c r="C31" s="8"/>
+      <c r="D31" s="8"/>
+      <c r="E31" s="8"/>
+      <c r="F31" s="8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1617,11 +1695,11 @@
       <c r="A32" s="1">
         <v>31</v>
       </c>
-      <c r="B32" s="10"/>
-      <c r="C32" s="10"/>
-      <c r="D32" s="10"/>
-      <c r="E32" s="10"/>
-      <c r="F32" s="10">
+      <c r="B32" s="8"/>
+      <c r="C32" s="8"/>
+      <c r="D32" s="8"/>
+      <c r="E32" s="8"/>
+      <c r="F32" s="8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1630,11 +1708,11 @@
       <c r="A33" s="1">
         <v>32</v>
       </c>
-      <c r="B33" s="10"/>
-      <c r="C33" s="10"/>
-      <c r="D33" s="10"/>
-      <c r="E33" s="10"/>
-      <c r="F33" s="10">
+      <c r="B33" s="8"/>
+      <c r="C33" s="8"/>
+      <c r="D33" s="8"/>
+      <c r="E33" s="8"/>
+      <c r="F33" s="8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1643,11 +1721,11 @@
       <c r="A34" s="1">
         <v>33</v>
       </c>
-      <c r="B34" s="10"/>
-      <c r="C34" s="10"/>
-      <c r="D34" s="10"/>
-      <c r="E34" s="10"/>
-      <c r="F34" s="10">
+      <c r="B34" s="8"/>
+      <c r="C34" s="8"/>
+      <c r="D34" s="8"/>
+      <c r="E34" s="8"/>
+      <c r="F34" s="8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1656,11 +1734,11 @@
       <c r="A35" s="1">
         <v>34</v>
       </c>
-      <c r="B35" s="10"/>
-      <c r="C35" s="10"/>
-      <c r="D35" s="10"/>
-      <c r="E35" s="10"/>
-      <c r="F35" s="10">
+      <c r="B35" s="8"/>
+      <c r="C35" s="8"/>
+      <c r="D35" s="8"/>
+      <c r="E35" s="8"/>
+      <c r="F35" s="8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1669,11 +1747,11 @@
       <c r="A36" s="1">
         <v>35</v>
       </c>
-      <c r="B36" s="10"/>
-      <c r="C36" s="10"/>
-      <c r="D36" s="10"/>
-      <c r="E36" s="10"/>
-      <c r="F36" s="10">
+      <c r="B36" s="8"/>
+      <c r="C36" s="8"/>
+      <c r="D36" s="8"/>
+      <c r="E36" s="8"/>
+      <c r="F36" s="8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1682,11 +1760,11 @@
       <c r="A37" s="1">
         <v>36</v>
       </c>
-      <c r="B37" s="10"/>
-      <c r="C37" s="10"/>
-      <c r="D37" s="10"/>
-      <c r="E37" s="10"/>
-      <c r="F37" s="10">
+      <c r="B37" s="8"/>
+      <c r="C37" s="8"/>
+      <c r="D37" s="8"/>
+      <c r="E37" s="8"/>
+      <c r="F37" s="8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1695,11 +1773,11 @@
       <c r="A38" s="1">
         <v>37</v>
       </c>
-      <c r="B38" s="10"/>
-      <c r="C38" s="10"/>
-      <c r="D38" s="10"/>
-      <c r="E38" s="10"/>
-      <c r="F38" s="10">
+      <c r="B38" s="8"/>
+      <c r="C38" s="8"/>
+      <c r="D38" s="8"/>
+      <c r="E38" s="8"/>
+      <c r="F38" s="8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1708,11 +1786,11 @@
       <c r="A39" s="1">
         <v>38</v>
       </c>
-      <c r="B39" s="10"/>
-      <c r="C39" s="10"/>
-      <c r="D39" s="10"/>
-      <c r="E39" s="10"/>
-      <c r="F39" s="10">
+      <c r="B39" s="8"/>
+      <c r="C39" s="8"/>
+      <c r="D39" s="8"/>
+      <c r="E39" s="8"/>
+      <c r="F39" s="8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1721,11 +1799,11 @@
       <c r="A40" s="1">
         <v>39</v>
       </c>
-      <c r="B40" s="10"/>
-      <c r="C40" s="10"/>
-      <c r="D40" s="10"/>
-      <c r="E40" s="10"/>
-      <c r="F40" s="10">
+      <c r="B40" s="8"/>
+      <c r="C40" s="8"/>
+      <c r="D40" s="8"/>
+      <c r="E40" s="8"/>
+      <c r="F40" s="8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1734,11 +1812,11 @@
       <c r="A41" s="1">
         <v>40</v>
       </c>
-      <c r="B41" s="10"/>
-      <c r="C41" s="10"/>
-      <c r="D41" s="10"/>
-      <c r="E41" s="10"/>
-      <c r="F41" s="10">
+      <c r="B41" s="8"/>
+      <c r="C41" s="8"/>
+      <c r="D41" s="8"/>
+      <c r="E41" s="8"/>
+      <c r="F41" s="8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1747,11 +1825,11 @@
       <c r="A42" s="1">
         <v>41</v>
       </c>
-      <c r="B42" s="10"/>
-      <c r="C42" s="10"/>
-      <c r="D42" s="10"/>
-      <c r="E42" s="10"/>
-      <c r="F42" s="10">
+      <c r="B42" s="8"/>
+      <c r="C42" s="8"/>
+      <c r="D42" s="8"/>
+      <c r="E42" s="8"/>
+      <c r="F42" s="8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1760,11 +1838,11 @@
       <c r="A43" s="1">
         <v>42</v>
       </c>
-      <c r="B43" s="10"/>
-      <c r="C43" s="10"/>
-      <c r="D43" s="10"/>
-      <c r="E43" s="10"/>
-      <c r="F43" s="10">
+      <c r="B43" s="8"/>
+      <c r="C43" s="8"/>
+      <c r="D43" s="8"/>
+      <c r="E43" s="8"/>
+      <c r="F43" s="8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1773,11 +1851,11 @@
       <c r="A44" s="1">
         <v>43</v>
       </c>
-      <c r="B44" s="10"/>
-      <c r="C44" s="10"/>
-      <c r="D44" s="10"/>
-      <c r="E44" s="10"/>
-      <c r="F44" s="10">
+      <c r="B44" s="8"/>
+      <c r="C44" s="8"/>
+      <c r="D44" s="8"/>
+      <c r="E44" s="8"/>
+      <c r="F44" s="8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1786,11 +1864,11 @@
       <c r="A45" s="1">
         <v>44</v>
       </c>
-      <c r="B45" s="10"/>
-      <c r="C45" s="10"/>
-      <c r="D45" s="10"/>
-      <c r="E45" s="10"/>
-      <c r="F45" s="10">
+      <c r="B45" s="8"/>
+      <c r="C45" s="8"/>
+      <c r="D45" s="8"/>
+      <c r="E45" s="8"/>
+      <c r="F45" s="8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1799,11 +1877,11 @@
       <c r="A46" s="1">
         <v>45</v>
       </c>
-      <c r="B46" s="10"/>
-      <c r="C46" s="10"/>
-      <c r="D46" s="10"/>
-      <c r="E46" s="10"/>
-      <c r="F46" s="10">
+      <c r="B46" s="8"/>
+      <c r="C46" s="8"/>
+      <c r="D46" s="8"/>
+      <c r="E46" s="8"/>
+      <c r="F46" s="8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1812,11 +1890,11 @@
       <c r="A47" s="1">
         <v>46</v>
       </c>
-      <c r="B47" s="10"/>
-      <c r="C47" s="10"/>
-      <c r="D47" s="10"/>
-      <c r="E47" s="10"/>
-      <c r="F47" s="10">
+      <c r="B47" s="8"/>
+      <c r="C47" s="8"/>
+      <c r="D47" s="8"/>
+      <c r="E47" s="8"/>
+      <c r="F47" s="8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1825,11 +1903,11 @@
       <c r="A48" s="1">
         <v>47</v>
       </c>
-      <c r="B48" s="10"/>
-      <c r="C48" s="10"/>
-      <c r="D48" s="10"/>
-      <c r="E48" s="10"/>
-      <c r="F48" s="10">
+      <c r="B48" s="8"/>
+      <c r="C48" s="8"/>
+      <c r="D48" s="8"/>
+      <c r="E48" s="8"/>
+      <c r="F48" s="8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1838,11 +1916,11 @@
       <c r="A49" s="1">
         <v>48</v>
       </c>
-      <c r="B49" s="10"/>
-      <c r="C49" s="10"/>
-      <c r="D49" s="10"/>
-      <c r="E49" s="10"/>
-      <c r="F49" s="10">
+      <c r="B49" s="8"/>
+      <c r="C49" s="8"/>
+      <c r="D49" s="8"/>
+      <c r="E49" s="8"/>
+      <c r="F49" s="8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1851,11 +1929,11 @@
       <c r="A50" s="1">
         <v>49</v>
       </c>
-      <c r="B50" s="10"/>
-      <c r="C50" s="10"/>
-      <c r="D50" s="10"/>
-      <c r="E50" s="10"/>
-      <c r="F50" s="10">
+      <c r="B50" s="8"/>
+      <c r="C50" s="8"/>
+      <c r="D50" s="8"/>
+      <c r="E50" s="8"/>
+      <c r="F50" s="8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1864,11 +1942,11 @@
       <c r="A51" s="1">
         <v>50</v>
       </c>
-      <c r="B51" s="10"/>
-      <c r="C51" s="10"/>
-      <c r="D51" s="10"/>
-      <c r="E51" s="10"/>
-      <c r="F51" s="10">
+      <c r="B51" s="8"/>
+      <c r="C51" s="8"/>
+      <c r="D51" s="8"/>
+      <c r="E51" s="8"/>
+      <c r="F51" s="8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1877,11 +1955,11 @@
       <c r="A52" s="1">
         <v>51</v>
       </c>
-      <c r="B52" s="10"/>
-      <c r="C52" s="10"/>
-      <c r="D52" s="10"/>
-      <c r="E52" s="10"/>
-      <c r="F52" s="10">
+      <c r="B52" s="8"/>
+      <c r="C52" s="8"/>
+      <c r="D52" s="8"/>
+      <c r="E52" s="8"/>
+      <c r="F52" s="8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1890,11 +1968,11 @@
       <c r="A53" s="1">
         <v>52</v>
       </c>
-      <c r="B53" s="10"/>
-      <c r="C53" s="10"/>
-      <c r="D53" s="10"/>
-      <c r="E53" s="10"/>
-      <c r="F53" s="10">
+      <c r="B53" s="8"/>
+      <c r="C53" s="8"/>
+      <c r="D53" s="8"/>
+      <c r="E53" s="8"/>
+      <c r="F53" s="8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1903,11 +1981,11 @@
       <c r="A54" s="1">
         <v>53</v>
       </c>
-      <c r="B54" s="10"/>
-      <c r="C54" s="10"/>
-      <c r="D54" s="10"/>
-      <c r="E54" s="10"/>
-      <c r="F54" s="10">
+      <c r="B54" s="8"/>
+      <c r="C54" s="8"/>
+      <c r="D54" s="8"/>
+      <c r="E54" s="8"/>
+      <c r="F54" s="8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1916,38 +1994,38 @@
       <c r="A55" s="1">
         <v>54</v>
       </c>
-      <c r="B55" s="10"/>
-      <c r="C55" s="10"/>
-      <c r="D55" s="10"/>
-      <c r="E55" s="10"/>
-      <c r="F55" s="10">
+      <c r="B55" s="8"/>
+      <c r="C55" s="8"/>
+      <c r="D55" s="8"/>
+      <c r="E55" s="8"/>
+      <c r="F55" s="8">
         <f xml:space="preserve"> SUM(B55, C55, D55, E55)</f>
         <v>0</v>
       </c>
     </row>
     <row r="56" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B56" s="10">
+        <v>29</v>
+      </c>
+      <c r="B56" s="8">
         <f xml:space="preserve"> AVERAGE(B2:B55)</f>
         <v>20</v>
       </c>
-      <c r="C56" s="10">
-        <f t="shared" ref="C56:F56" si="1" xml:space="preserve"> AVERAGE(C2:C55)</f>
-        <v>21</v>
-      </c>
-      <c r="D56" s="10">
+      <c r="C56" s="8">
+        <f t="shared" ref="C56:E56" si="1" xml:space="preserve"> AVERAGE(C2:C55)</f>
+        <v>23</v>
+      </c>
+      <c r="D56" s="8">
         <f t="shared" si="1"/>
         <v>20</v>
       </c>
-      <c r="E56" s="10">
+      <c r="E56" s="8">
         <f t="shared" si="1"/>
         <v>20</v>
       </c>
-      <c r="F56" s="10">
+      <c r="F56" s="8">
         <f xml:space="preserve"> SUM(B56, C56, D56, E56)</f>
-        <v>81</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add memrise dictionaries and update my progress
</commit_message>
<xml_diff>
--- a/TOEFL/Progress.xlsx
+++ b/TOEFL/Progress.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="7020" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="8190" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Progree" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="53">
   <si>
     <t>Book/CD Name</t>
   </si>
@@ -140,6 +140,45 @@
   </si>
   <si>
     <t>Review Words Flash Cards</t>
+  </si>
+  <si>
+    <t>Memrise / 400 Words for TOEFL Intermediate</t>
+  </si>
+  <si>
+    <t>Memrise / 50 Basic Roots for English</t>
+  </si>
+  <si>
+    <t>Memrise / 1100 Words you need to know</t>
+  </si>
+  <si>
+    <t>Memrise / English Expressions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Memrise / Important Vocabs for TOEFL IBT </t>
+  </si>
+  <si>
+    <t>Memrise / 350 Idioms, Sayings and Slang</t>
+  </si>
+  <si>
+    <t>Memrise / Advanced English for Native Speakers</t>
+  </si>
+  <si>
+    <t>Memrise / Learn English Irregular Verbs</t>
+  </si>
+  <si>
+    <t>Memrise / 4000 Words for Educated Vocab</t>
+  </si>
+  <si>
+    <t>Memrise / Essential Words for the TOEFL (6th)</t>
+  </si>
+  <si>
+    <t>Memrise / 504 Absolutely Essential Words</t>
+  </si>
+  <si>
+    <t>Memrise / 1212 Words you need to know</t>
+  </si>
+  <si>
+    <t>Memrise / TOEFL Vocabularies by Zhan</t>
   </si>
 </sst>
 </file>
@@ -344,8 +383,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A2:J24" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18">
-  <autoFilter ref="A2:J24"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A2:J37" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18">
+  <autoFilter ref="A2:J37"/>
   <tableColumns count="10">
     <tableColumn id="1" name="No." dataDxfId="17"/>
     <tableColumn id="2" name="Book/CD Name" dataDxfId="16"/>
@@ -644,10 +683,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J25"/>
+  <dimension ref="A1:J38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="I26" sqref="I26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -768,7 +807,7 @@
       </c>
     </row>
     <row r="5" spans="1:10" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
+      <c r="A5" s="9">
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -1218,23 +1257,402 @@
         <v>22</v>
       </c>
       <c r="B24" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="C24" s="9">
+        <v>400</v>
+      </c>
+      <c r="D24" s="9">
+        <v>40</v>
+      </c>
+      <c r="E24" s="11" t="str">
+        <f xml:space="preserve"> CONCATENATE(CEILING(Table1[[#This Row],[Current Part/Page]]/Table1[[#This Row],[Part/Page count]], 0.0001) * 100,"%")</f>
+        <v>10%</v>
+      </c>
+      <c r="F24" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="G24" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="H24" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="I24" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="J24" s="9"/>
+    </row>
+    <row r="25" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="9">
+        <v>23</v>
+      </c>
+      <c r="B25" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="C25" s="9">
+        <v>50</v>
+      </c>
+      <c r="D25" s="9"/>
+      <c r="E25" s="11" t="str">
+        <f xml:space="preserve"> CONCATENATE(CEILING(Table1[[#This Row],[Current Part/Page]]/Table1[[#This Row],[Part/Page count]], 0.0001) * 100,"%")</f>
+        <v>0%</v>
+      </c>
+      <c r="F25" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="G25" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="H25" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="I25" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="J25" s="9"/>
+    </row>
+    <row r="26" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="9">
+        <v>24</v>
+      </c>
+      <c r="B26" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="C26" s="9">
+        <v>1100</v>
+      </c>
+      <c r="D26" s="9"/>
+      <c r="E26" s="11" t="str">
+        <f xml:space="preserve"> CONCATENATE(CEILING(Table1[[#This Row],[Current Part/Page]]/Table1[[#This Row],[Part/Page count]], 0.0001) * 100,"%")</f>
+        <v>0%</v>
+      </c>
+      <c r="F26" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="G26" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="H26" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="I26" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="J26" s="9"/>
+    </row>
+    <row r="27" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="9">
+        <v>25</v>
+      </c>
+      <c r="B27" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="C27" s="9">
+        <v>600</v>
+      </c>
+      <c r="D27" s="9"/>
+      <c r="E27" s="11" t="str">
+        <f xml:space="preserve"> CONCATENATE(CEILING(Table1[[#This Row],[Current Part/Page]]/Table1[[#This Row],[Part/Page count]], 0.0001) * 100,"%")</f>
+        <v>0%</v>
+      </c>
+      <c r="F27" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="G27" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="H27" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="I27" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="J27" s="9"/>
+    </row>
+    <row r="28" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="9">
+        <v>26</v>
+      </c>
+      <c r="B28" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="C28" s="9">
+        <v>684</v>
+      </c>
+      <c r="D28" s="9"/>
+      <c r="E28" s="11" t="str">
+        <f xml:space="preserve"> CONCATENATE(CEILING(Table1[[#This Row],[Current Part/Page]]/Table1[[#This Row],[Part/Page count]], 0.0001) * 100,"%")</f>
+        <v>0%</v>
+      </c>
+      <c r="F28" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="G28" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="H28" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="I28" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="J28" s="9"/>
+    </row>
+    <row r="29" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="9">
+        <v>27</v>
+      </c>
+      <c r="B29" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C29" s="9">
+        <v>117</v>
+      </c>
+      <c r="D29" s="9"/>
+      <c r="E29" s="11" t="str">
+        <f xml:space="preserve"> CONCATENATE(CEILING(Table1[[#This Row],[Current Part/Page]]/Table1[[#This Row],[Part/Page count]], 0.0001) * 100,"%")</f>
+        <v>0%</v>
+      </c>
+      <c r="F29" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="G29" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="H29" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="I29" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="J29" s="9"/>
+    </row>
+    <row r="30" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="9">
+        <v>28</v>
+      </c>
+      <c r="B30" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="C30" s="9">
+        <v>1122</v>
+      </c>
+      <c r="D30" s="9"/>
+      <c r="E30" s="11" t="str">
+        <f xml:space="preserve"> CONCATENATE(CEILING(Table1[[#This Row],[Current Part/Page]]/Table1[[#This Row],[Part/Page count]], 0.0001) * 100,"%")</f>
+        <v>0%</v>
+      </c>
+      <c r="F30" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="G30" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="H30" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="I30" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="J30" s="9"/>
+    </row>
+    <row r="31" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="9">
+        <v>29</v>
+      </c>
+      <c r="B31" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="C31" s="9">
+        <v>375</v>
+      </c>
+      <c r="D31" s="9"/>
+      <c r="E31" s="11" t="str">
+        <f xml:space="preserve"> CONCATENATE(CEILING(Table1[[#This Row],[Current Part/Page]]/Table1[[#This Row],[Part/Page count]], 0.0001) * 100,"%")</f>
+        <v>0%</v>
+      </c>
+      <c r="F31" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="G31" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="H31" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="I31" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="J31" s="9"/>
+    </row>
+    <row r="32" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="9">
+        <v>30</v>
+      </c>
+      <c r="B32" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="C32" s="9">
+        <v>550</v>
+      </c>
+      <c r="D32" s="9"/>
+      <c r="E32" s="11" t="str">
+        <f xml:space="preserve"> CONCATENATE(CEILING(Table1[[#This Row],[Current Part/Page]]/Table1[[#This Row],[Part/Page count]], 0.0001) * 100,"%")</f>
+        <v>0%</v>
+      </c>
+      <c r="F32" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="G32" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="H32" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="I32" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="J32" s="9"/>
+    </row>
+    <row r="33" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="9">
+        <v>31</v>
+      </c>
+      <c r="B33" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="C33" s="9">
+        <v>504</v>
+      </c>
+      <c r="D33" s="9"/>
+      <c r="E33" s="11" t="str">
+        <f xml:space="preserve"> CONCATENATE(CEILING(Table1[[#This Row],[Current Part/Page]]/Table1[[#This Row],[Part/Page count]], 0.0001) * 100,"%")</f>
+        <v>0%</v>
+      </c>
+      <c r="F33" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="G33" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="H33" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="I33" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="J33" s="9"/>
+    </row>
+    <row r="34" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="9">
+        <v>32</v>
+      </c>
+      <c r="B34" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="C34" s="9">
+        <v>1321</v>
+      </c>
+      <c r="D34" s="9"/>
+      <c r="E34" s="11" t="str">
+        <f xml:space="preserve"> CONCATENATE(CEILING(Table1[[#This Row],[Current Part/Page]]/Table1[[#This Row],[Part/Page count]], 0.0001) * 100,"%")</f>
+        <v>0%</v>
+      </c>
+      <c r="F34" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="G34" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="H34" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="I34" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="J34" s="9"/>
+    </row>
+    <row r="35" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="9">
+        <v>33</v>
+      </c>
+      <c r="B35" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="C35" s="9">
+        <v>400</v>
+      </c>
+      <c r="D35" s="9"/>
+      <c r="E35" s="11" t="str">
+        <f xml:space="preserve"> CONCATENATE(CEILING(Table1[[#This Row],[Current Part/Page]]/Table1[[#This Row],[Part/Page count]], 0.0001) * 100,"%")</f>
+        <v>0%</v>
+      </c>
+      <c r="F35" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="G35" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="H35" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="I35" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="J35" s="9"/>
+    </row>
+    <row r="36" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="9">
         <v>34</v>
       </c>
-      <c r="C24" s="9">
+      <c r="B36" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="C36" s="9">
+        <v>1100</v>
+      </c>
+      <c r="D36" s="9"/>
+      <c r="E36" s="11" t="str">
+        <f xml:space="preserve"> CONCATENATE(CEILING(Table1[[#This Row],[Current Part/Page]]/Table1[[#This Row],[Part/Page count]], 0.0001) * 100,"%")</f>
+        <v>0%</v>
+      </c>
+      <c r="F36" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="G36" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="H36" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="I36" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="J36" s="9"/>
+    </row>
+    <row r="37" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="9">
+        <v>35</v>
+      </c>
+      <c r="B37" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="C37" s="9">
         <v>200</v>
       </c>
-      <c r="D24" s="9"/>
-      <c r="E24" s="11" t="str">
-        <f xml:space="preserve"> CONCATENATE(CEILING(Table1[[#This Row],[Current Part/Page]]/Table1[[#This Row],[Part/Page count]], 0.0001) * 100,"%")</f>
-        <v>0%</v>
-      </c>
-      <c r="F24" s="9"/>
-      <c r="G24" s="9"/>
-      <c r="H24" s="9"/>
-      <c r="I24" s="9"/>
-      <c r="J24" s="9"/>
-    </row>
-    <row r="25" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="D37" s="9"/>
+      <c r="E37" s="11" t="str">
+        <f xml:space="preserve"> CONCATENATE(CEILING(Table1[[#This Row],[Current Part/Page]]/Table1[[#This Row],[Part/Page count]], 0.0001) * 100,"%")</f>
+        <v>0%</v>
+      </c>
+      <c r="F37" s="9"/>
+      <c r="G37" s="9"/>
+      <c r="H37" s="9"/>
+      <c r="I37" s="9"/>
+      <c r="J37" s="9"/>
+    </row>
+    <row r="38" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="F1:I1"/>

</xml_diff>

<commit_message>
Update TOEFL Progress after so many days!
</commit_message>
<xml_diff>
--- a/TOEFL/Progress.xlsx
+++ b/TOEFL/Progress.xlsx
@@ -4,10 +4,10 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="9360" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="14040" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Progree" sheetId="1" r:id="rId1"/>
+    <sheet name="Progress" sheetId="1" r:id="rId1"/>
     <sheet name="TPO Results" sheetId="4" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="53">
   <si>
     <t>Book/CD Name</t>
   </si>
@@ -175,10 +175,10 @@
     <t>Memrise / TOEFL Vocabularies by Zhan</t>
   </si>
   <si>
-    <t>17, 28, 29, 34, 36</t>
-  </si>
-  <si>
-    <t>1.5, 2.7, 3.7</t>
+    <t>17, 28, 29, 34, 36, 60, 74</t>
+  </si>
+  <si>
+    <t>1.5, 2.7, 3.7, 6.1, 6.7</t>
   </si>
 </sst>
 </file>
@@ -685,8 +685,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -751,14 +751,14 @@
         <v>2</v>
       </c>
       <c r="C3" s="1">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D3" s="1">
-        <v>4.3</v>
+        <v>7.1</v>
       </c>
       <c r="E3" s="5" t="str">
         <f xml:space="preserve"> CONCATENATE(CEILING(Table1[[#This Row],[Current Part/Page]]/Table1[[#This Row],[Part/Page count]], 0.0001) * 100,"%")</f>
-        <v>25.3%</v>
+        <v>39.45%</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>17</v>
@@ -787,11 +787,11 @@
         <v>310</v>
       </c>
       <c r="D4" s="1">
-        <v>49</v>
+        <v>83</v>
       </c>
       <c r="E4" s="5" t="str">
         <f xml:space="preserve"> CONCATENATE(CEILING(Table1[[#This Row],[Current Part/Page]]/Table1[[#This Row],[Part/Page count]], 0.0001) * 100,"%")</f>
-        <v>15.81%</v>
+        <v>26.78%</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>17</v>
@@ -842,7 +842,9 @@
         <f xml:space="preserve"> CONCATENATE(CEILING(Table1[[#This Row],[Current Part/Page]]/Table1[[#This Row],[Part/Page count]], 0.0001) * 100,"%")</f>
         <v>0%</v>
       </c>
-      <c r="I6" s="10"/>
+      <c r="I6" s="10" t="s">
+        <v>17</v>
+      </c>
       <c r="J6" s="10"/>
     </row>
     <row r="7" spans="1:10" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1086,7 +1088,9 @@
         <f xml:space="preserve"> CONCATENATE(CEILING(Table1[[#This Row],[Current Part/Page]]/Table1[[#This Row],[Part/Page count]], 0.0001) * 100,"%")</f>
         <v>0%</v>
       </c>
-      <c r="F16" s="1"/>
+      <c r="F16" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
@@ -1110,7 +1114,9 @@
         <v>5%</v>
       </c>
       <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
+      <c r="G17" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
@@ -1132,7 +1138,9 @@
       </c>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
-      <c r="H18" s="1"/>
+      <c r="H18" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
     </row>
@@ -1151,14 +1159,12 @@
         <f xml:space="preserve"> CONCATENATE(CEILING(Table1[[#This Row],[Current Part/Page]]/Table1[[#This Row],[Part/Page count]], 0.0001) * 100,"%")</f>
         <v>0%</v>
       </c>
-      <c r="F19" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>17</v>
-      </c>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
       <c r="H19" s="1"/>
-      <c r="I19" s="1"/>
+      <c r="I19" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="J19" s="1"/>
     </row>
     <row r="20" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1254,7 +1260,9 @@
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
-      <c r="I23" s="1"/>
+      <c r="I23" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="J23" s="1"/>
     </row>
     <row r="24" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1268,11 +1276,11 @@
         <v>400</v>
       </c>
       <c r="D24" s="9">
-        <v>140</v>
+        <v>200</v>
       </c>
       <c r="E24" s="11" t="str">
         <f xml:space="preserve"> CONCATENATE(CEILING(Table1[[#This Row],[Current Part/Page]]/Table1[[#This Row],[Part/Page count]], 0.0001) * 100,"%")</f>
-        <v>35%</v>
+        <v>50%</v>
       </c>
       <c r="F24" s="10" t="s">
         <v>17</v>
@@ -1657,8 +1665,12 @@
       </c>
       <c r="F37" s="9"/>
       <c r="G37" s="9"/>
-      <c r="H37" s="9"/>
-      <c r="I37" s="9"/>
+      <c r="H37" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="I37" s="9" t="s">
+        <v>17</v>
+      </c>
       <c r="J37" s="9"/>
     </row>
     <row r="38" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1678,8 +1690,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J56"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C46" sqref="C46"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Update Progress and add Idioms and Words
</commit_message>
<xml_diff>
--- a/TOEFL/Progress.xlsx
+++ b/TOEFL/Progress.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="0" windowWidth="19320" windowHeight="8205"/>
+    <workbookView xWindow="9360" yWindow="0" windowWidth="16980" windowHeight="8205"/>
   </bookViews>
   <sheets>
     <sheet name="Progress" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="61">
   <si>
     <t>Book/CD Name</t>
   </si>
@@ -185,6 +185,24 @@
   </si>
   <si>
     <t>19-24, 39-40, 43, 45-49, 69</t>
+  </si>
+  <si>
+    <t>Vocabulary and Grammar for the TOEFL - Collins</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Review the copied pages </t>
+  </si>
+  <si>
+    <t>Word Power Made Easy</t>
+  </si>
+  <si>
+    <t>TED-Ed videos</t>
+  </si>
+  <si>
+    <t>BBC Learning English Towards Advanced Course</t>
+  </si>
+  <si>
+    <t>Grammar Booster</t>
   </si>
 </sst>
 </file>
@@ -389,8 +407,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A2:J38" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18">
-  <autoFilter ref="A2:J38"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A2:J43" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18">
+  <autoFilter ref="A2:J43"/>
   <tableColumns count="10">
     <tableColumn id="1" name="No." dataDxfId="17"/>
     <tableColumn id="2" name="Book/CD Name" dataDxfId="16"/>
@@ -689,10 +707,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J39"/>
+  <dimension ref="A1:J44"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" topLeftCell="A35" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D41" sqref="D41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -917,11 +935,11 @@
         <v>550</v>
       </c>
       <c r="D9" s="1">
-        <v>153</v>
+        <v>234</v>
       </c>
       <c r="E9" s="5" t="str">
         <f xml:space="preserve"> CONCATENATE(CEILING(Table1[[#This Row],[Current Part/Page]]/Table1[[#This Row],[Part/Page count]], 0.0001) * 100,"%")</f>
-        <v>27.82%</v>
+        <v>42.55%</v>
       </c>
       <c r="F9" s="3" t="s">
         <v>16</v>
@@ -948,11 +966,11 @@
         <v>500</v>
       </c>
       <c r="D10" s="9">
-        <v>253</v>
+        <v>434</v>
       </c>
       <c r="E10" s="11" t="str">
         <f xml:space="preserve"> CONCATENATE(CEILING(Table1[[#This Row],[Current Part/Page]]/Table1[[#This Row],[Part/Page count]], 0.0001) * 100,"%")</f>
-        <v>50.6%</v>
+        <v>86.8%</v>
       </c>
       <c r="F10" s="10" t="s">
         <v>16</v>
@@ -1090,11 +1108,11 @@
         <v>60</v>
       </c>
       <c r="D16" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E16" s="5" t="str">
         <f xml:space="preserve"> CONCATENATE(CEILING(Table1[[#This Row],[Current Part/Page]]/Table1[[#This Row],[Part/Page count]], 0.0001) * 100,"%")</f>
-        <v>6.67%</v>
+        <v>8.34%</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>16</v>
@@ -1187,12 +1205,14 @@
         <v>53</v>
       </c>
       <c r="C20" s="1">
-        <v>64</v>
-      </c>
-      <c r="D20" s="1"/>
+        <v>52</v>
+      </c>
+      <c r="D20" s="1">
+        <v>42</v>
+      </c>
       <c r="E20" s="5" t="str">
         <f xml:space="preserve"> CONCATENATE(CEILING(Table1[[#This Row],[Current Part/Page]]/Table1[[#This Row],[Part/Page count]], 0.0001) * 100,"%")</f>
-        <v>0%</v>
+        <v>80.77%</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>16</v>
@@ -1694,27 +1714,168 @@
         <v>36</v>
       </c>
       <c r="B38" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="C38" s="9">
+        <v>170</v>
+      </c>
+      <c r="D38" s="9">
+        <v>108</v>
+      </c>
+      <c r="E38" s="11" t="str">
+        <f xml:space="preserve"> CONCATENATE(CEILING(Table1[[#This Row],[Current Part/Page]]/Table1[[#This Row],[Part/Page count]], 0.0001) * 100,"%")</f>
+        <v>63.53%</v>
+      </c>
+      <c r="F38" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="G38" s="10"/>
+      <c r="H38" s="10"/>
+      <c r="I38" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="J38" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="9">
+        <v>37</v>
+      </c>
+      <c r="B39" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="C39" s="9">
+        <v>100</v>
+      </c>
+      <c r="D39" s="9">
+        <v>0</v>
+      </c>
+      <c r="E39" s="11" t="str">
+        <f xml:space="preserve"> CONCATENATE(CEILING(Table1[[#This Row],[Current Part/Page]]/Table1[[#This Row],[Part/Page count]], 0.0001) * 100,"%")</f>
+        <v>0%</v>
+      </c>
+      <c r="F39" s="10"/>
+      <c r="G39" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="H39" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="I39" s="10"/>
+      <c r="J39" s="9"/>
+    </row>
+    <row r="40" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="9">
+        <v>38</v>
+      </c>
+      <c r="B40" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="C40" s="9">
+        <v>528</v>
+      </c>
+      <c r="D40" s="9">
+        <v>70</v>
+      </c>
+      <c r="E40" s="11" t="str">
+        <f xml:space="preserve"> CONCATENATE(CEILING(Table1[[#This Row],[Current Part/Page]]/Table1[[#This Row],[Part/Page count]], 0.0001) * 100,"%")</f>
+        <v>13.26%</v>
+      </c>
+      <c r="F40" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="G40" s="10"/>
+      <c r="H40" s="10"/>
+      <c r="I40" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="J40" s="9"/>
+    </row>
+    <row r="41" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="9">
+        <v>39</v>
+      </c>
+      <c r="B41" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="C41" s="9">
+        <v>30</v>
+      </c>
+      <c r="D41" s="9">
+        <v>2</v>
+      </c>
+      <c r="E41" s="11" t="str">
+        <f xml:space="preserve"> CONCATENATE(CEILING(Table1[[#This Row],[Current Part/Page]]/Table1[[#This Row],[Part/Page count]], 0.0001) * 100,"%")</f>
+        <v>6.67%</v>
+      </c>
+      <c r="F41" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="G41" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="H41" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="I41" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="J41" s="9"/>
+    </row>
+    <row r="42" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="9">
+        <v>40</v>
+      </c>
+      <c r="B42" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="C42" s="9">
+        <v>120</v>
+      </c>
+      <c r="D42" s="9">
+        <v>10</v>
+      </c>
+      <c r="E42" s="11" t="str">
+        <f xml:space="preserve"> CONCATENATE(CEILING(Table1[[#This Row],[Current Part/Page]]/Table1[[#This Row],[Part/Page count]], 0.0001) * 100,"%")</f>
+        <v>8.34%</v>
+      </c>
+      <c r="F42" s="10"/>
+      <c r="G42" s="10"/>
+      <c r="H42" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="I42" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="J42" s="9"/>
+    </row>
+    <row r="43" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="9">
+        <v>41</v>
+      </c>
+      <c r="B43" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="C38" s="9">
+      <c r="C43" s="9">
         <v>200</v>
       </c>
-      <c r="D38" s="9"/>
-      <c r="E38" s="11" t="str">
+      <c r="D43" s="9"/>
+      <c r="E43" s="11" t="str">
         <f xml:space="preserve"> CONCATENATE(CEILING(Table1[[#This Row],[Current Part/Page]]/Table1[[#This Row],[Part/Page count]], 0.0001) * 100,"%")</f>
         <v>0%</v>
       </c>
-      <c r="F38" s="9"/>
-      <c r="G38" s="9"/>
-      <c r="H38" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="I38" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="J38" s="9"/>
-    </row>
-    <row r="39" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="F43" s="9"/>
+      <c r="G43" s="9"/>
+      <c r="H43" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="I43" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="J43" s="9"/>
+    </row>
+    <row r="44" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="F1:I1"/>
@@ -1732,7 +1893,7 @@
   <dimension ref="A1:J56"/>
   <sheetViews>
     <sheetView topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="B42" sqref="B42"/>
+      <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2309,13 +2470,15 @@
       <c r="A42" s="1">
         <v>41</v>
       </c>
-      <c r="B42" s="8"/>
+      <c r="B42" s="8">
+        <v>23</v>
+      </c>
       <c r="C42" s="8"/>
       <c r="D42" s="8"/>
       <c r="E42" s="8"/>
       <c r="F42" s="8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>23</v>
       </c>
     </row>
     <row r="43" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2513,7 +2676,7 @@
       </c>
       <c r="B56" s="8">
         <f xml:space="preserve"> AVERAGE(B2:B55)</f>
-        <v>20.2</v>
+        <v>20.666666666666668</v>
       </c>
       <c r="C56" s="8">
         <f t="shared" ref="C56:E56" si="1" xml:space="preserve"> AVERAGE(C2:C55)</f>
@@ -2529,7 +2692,7 @@
       </c>
       <c r="F56" s="8">
         <f xml:space="preserve"> SUM(B56, C56, D56, E56)</f>
-        <v>84.45</v>
+        <v>84.916666666666671</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update idioms and words
</commit_message>
<xml_diff>
--- a/TOEFL/Progress.xlsx
+++ b/TOEFL/Progress.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="9360" yWindow="0" windowWidth="16980" windowHeight="8205"/>
+    <workbookView xWindow="12870" yWindow="0" windowWidth="16980" windowHeight="8205"/>
   </bookViews>
   <sheets>
     <sheet name="Progress" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="67">
   <si>
     <t>Book/CD Name</t>
   </si>
@@ -203,6 +203,24 @@
   </si>
   <si>
     <t>Grammar Booster</t>
+  </si>
+  <si>
+    <t>Topic-Specific Words</t>
+  </si>
+  <si>
+    <t>Needs Review</t>
+  </si>
+  <si>
+    <t>Review Words and idioms</t>
+  </si>
+  <si>
+    <t>English Collocations In Use - Intermediate</t>
+  </si>
+  <si>
+    <t>English Collocations In Use - Advanced</t>
+  </si>
+  <si>
+    <t>Check your vocabulary for TOEFL</t>
   </si>
 </sst>
 </file>
@@ -407,8 +425,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A2:J43" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18">
-  <autoFilter ref="A2:J43"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A2:J47" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18">
+  <autoFilter ref="A2:J47"/>
   <tableColumns count="10">
     <tableColumn id="1" name="No." dataDxfId="17"/>
     <tableColumn id="2" name="Book/CD Name" dataDxfId="16"/>
@@ -707,10 +725,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J44"/>
+  <dimension ref="A1:J48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D41" sqref="D41"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D43" sqref="D43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1746,14 +1764,14 @@
         <v>58</v>
       </c>
       <c r="C39" s="9">
-        <v>100</v>
+        <v>115</v>
       </c>
       <c r="D39" s="9">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="E39" s="11" t="str">
         <f xml:space="preserve"> CONCATENATE(CEILING(Table1[[#This Row],[Current Part/Page]]/Table1[[#This Row],[Part/Page count]], 0.0001) * 100,"%")</f>
-        <v>0%</v>
+        <v>24.35%</v>
       </c>
       <c r="F39" s="10"/>
       <c r="G39" s="10" t="s">
@@ -1763,7 +1781,9 @@
         <v>16</v>
       </c>
       <c r="I39" s="10"/>
-      <c r="J39" s="9"/>
+      <c r="J39" s="9" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="40" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="9">
@@ -1790,7 +1810,9 @@
       <c r="I40" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="J40" s="9"/>
+      <c r="J40" s="9" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="41" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="9">
@@ -1803,11 +1825,11 @@
         <v>30</v>
       </c>
       <c r="D41" s="9">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E41" s="11" t="str">
         <f xml:space="preserve"> CONCATENATE(CEILING(Table1[[#This Row],[Current Part/Page]]/Table1[[#This Row],[Part/Page count]], 0.0001) * 100,"%")</f>
-        <v>6.67%</v>
+        <v>13.34%</v>
       </c>
       <c r="F41" s="10" t="s">
         <v>16</v>
@@ -1821,7 +1843,9 @@
       <c r="I41" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="J41" s="9"/>
+      <c r="J41" s="9" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="42" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="9">
@@ -1834,11 +1858,11 @@
         <v>120</v>
       </c>
       <c r="D42" s="9">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="E42" s="11" t="str">
         <f xml:space="preserve"> CONCATENATE(CEILING(Table1[[#This Row],[Current Part/Page]]/Table1[[#This Row],[Part/Page count]], 0.0001) * 100,"%")</f>
-        <v>8.34%</v>
+        <v>12.5%</v>
       </c>
       <c r="F42" s="10"/>
       <c r="G42" s="10"/>
@@ -1855,27 +1879,149 @@
         <v>41</v>
       </c>
       <c r="B43" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="C43" s="9">
+        <v>80</v>
+      </c>
+      <c r="D43" s="9">
+        <v>29</v>
+      </c>
+      <c r="E43" s="11" t="str">
+        <f xml:space="preserve"> CONCATENATE(CEILING(Table1[[#This Row],[Current Part/Page]]/Table1[[#This Row],[Part/Page count]], 0.0001) * 100,"%")</f>
+        <v>36.25%</v>
+      </c>
+      <c r="F43" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="G43" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="H43" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="I43" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="J43" s="9" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="9">
+        <v>42</v>
+      </c>
+      <c r="B44" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="C44" s="9">
+        <v>190</v>
+      </c>
+      <c r="D44" s="9">
+        <v>10</v>
+      </c>
+      <c r="E44" s="11" t="str">
+        <f xml:space="preserve"> CONCATENATE(CEILING(Table1[[#This Row],[Current Part/Page]]/Table1[[#This Row],[Part/Page count]], 0.0001) * 100,"%")</f>
+        <v>5.27%</v>
+      </c>
+      <c r="F44" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="G44" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="H44" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="I44" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="J44" s="9"/>
+    </row>
+    <row r="45" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="9">
+        <v>43</v>
+      </c>
+      <c r="B45" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="C45" s="9">
+        <v>186</v>
+      </c>
+      <c r="D45" s="9"/>
+      <c r="E45" s="11" t="str">
+        <f xml:space="preserve"> CONCATENATE(CEILING(Table1[[#This Row],[Current Part/Page]]/Table1[[#This Row],[Part/Page count]], 0.0001) * 100,"%")</f>
+        <v>0%</v>
+      </c>
+      <c r="F45" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="G45" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="H45" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="I45" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="J45" s="9"/>
+    </row>
+    <row r="46" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="9">
+        <v>44</v>
+      </c>
+      <c r="B46" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="C46" s="9">
+        <v>130</v>
+      </c>
+      <c r="D46" s="9"/>
+      <c r="E46" s="11" t="str">
+        <f xml:space="preserve"> CONCATENATE(CEILING(Table1[[#This Row],[Current Part/Page]]/Table1[[#This Row],[Part/Page count]], 0.0001) * 100,"%")</f>
+        <v>0%</v>
+      </c>
+      <c r="F46" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="G46" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="H46" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="I46" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="J46" s="9"/>
+    </row>
+    <row r="47" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="9">
+        <v>42</v>
+      </c>
+      <c r="B47" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="C43" s="9">
+      <c r="C47" s="9">
         <v>200</v>
       </c>
-      <c r="D43" s="9"/>
-      <c r="E43" s="11" t="str">
+      <c r="D47" s="9"/>
+      <c r="E47" s="11" t="str">
         <f xml:space="preserve"> CONCATENATE(CEILING(Table1[[#This Row],[Current Part/Page]]/Table1[[#This Row],[Part/Page count]], 0.0001) * 100,"%")</f>
         <v>0%</v>
       </c>
-      <c r="F43" s="9"/>
-      <c r="G43" s="9"/>
-      <c r="H43" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="I43" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="J43" s="9"/>
-    </row>
-    <row r="44" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="F47" s="9"/>
+      <c r="G47" s="9"/>
+      <c r="H47" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="I47" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="J47" s="9"/>
+    </row>
+    <row r="48" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="F1:I1"/>

</xml_diff>

<commit_message>
update idioms, words and sentences
</commit_message>
<xml_diff>
--- a/TOEFL/Progress.xlsx
+++ b/TOEFL/Progress.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="12870" yWindow="0" windowWidth="16980" windowHeight="8205"/>
+    <workbookView xWindow="16380" yWindow="0" windowWidth="16980" windowHeight="8205"/>
   </bookViews>
   <sheets>
     <sheet name="Progress" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="63">
   <si>
     <t>Book/CD Name</t>
   </si>
@@ -92,18 +92,6 @@
   </si>
   <si>
     <t>Notefull Videos and Docs / Writing</t>
-  </si>
-  <si>
-    <t>TPO Tests / Reading</t>
-  </si>
-  <si>
-    <t>TPO Tests / Listening</t>
-  </si>
-  <si>
-    <t>TPO Tests / Speaking</t>
-  </si>
-  <si>
-    <t>TPO Tests / Writing</t>
   </si>
   <si>
     <t>AVG</t>
@@ -425,8 +413,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A2:J47" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18">
-  <autoFilter ref="A2:J47"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A2:J43" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18">
+  <autoFilter ref="A2:J43"/>
   <tableColumns count="10">
     <tableColumn id="1" name="No." dataDxfId="17"/>
     <tableColumn id="2" name="Book/CD Name" dataDxfId="16"/>
@@ -727,8 +715,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D43" sqref="D43"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -782,7 +770,7 @@
         <v>15</v>
       </c>
       <c r="J2" s="6" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:10" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -815,7 +803,7 @@
         <v>16</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:10" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -845,7 +833,7 @@
         <v>17</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:10" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -875,7 +863,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C6" s="9">
         <v>17</v>
@@ -953,11 +941,11 @@
         <v>550</v>
       </c>
       <c r="D9" s="1">
-        <v>234</v>
+        <v>550</v>
       </c>
       <c r="E9" s="5" t="str">
         <f xml:space="preserve"> CONCATENATE(CEILING(Table1[[#This Row],[Current Part/Page]]/Table1[[#This Row],[Part/Page count]], 0.0001) * 100,"%")</f>
-        <v>42.55%</v>
+        <v>100%</v>
       </c>
       <c r="F9" s="3" t="s">
         <v>16</v>
@@ -978,17 +966,17 @@
         <v>8</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C10" s="9">
         <v>500</v>
       </c>
       <c r="D10" s="9">
-        <v>434</v>
+        <v>440</v>
       </c>
       <c r="E10" s="11" t="str">
         <f xml:space="preserve"> CONCATENATE(CEILING(Table1[[#This Row],[Current Part/Page]]/Table1[[#This Row],[Part/Page count]], 0.0001) * 100,"%")</f>
-        <v>86.8%</v>
+        <v>88%</v>
       </c>
       <c r="F10" s="10" t="s">
         <v>16</v>
@@ -1120,23 +1108,25 @@
         <v>14</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>24</v>
+        <v>49</v>
       </c>
       <c r="C16" s="1">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="D16" s="1">
-        <v>5</v>
+        <v>52</v>
       </c>
       <c r="E16" s="5" t="str">
         <f xml:space="preserve"> CONCATENATE(CEILING(Table1[[#This Row],[Current Part/Page]]/Table1[[#This Row],[Part/Page count]], 0.0001) * 100,"%")</f>
-        <v>8.34%</v>
+        <v>100%</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
+      <c r="G16" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H16" s="3"/>
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
     </row>
@@ -1145,24 +1135,24 @@
         <v>15</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="C17" s="1">
-        <v>60</v>
-      </c>
-      <c r="D17" s="1">
-        <v>8</v>
-      </c>
+        <v>170</v>
+      </c>
+      <c r="D17" s="1"/>
       <c r="E17" s="5" t="str">
         <f xml:space="preserve"> CONCATENATE(CEILING(Table1[[#This Row],[Current Part/Page]]/Table1[[#This Row],[Part/Page count]], 0.0001) * 100,"%")</f>
-        <v>13.34%</v>
-      </c>
-      <c r="F17" s="1"/>
-      <c r="G17" s="1" t="s">
-        <v>16</v>
-      </c>
+        <v>0%</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G17" s="1"/>
       <c r="H17" s="1"/>
-      <c r="I17" s="1"/>
+      <c r="I17" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="J17" s="1"/>
     </row>
     <row r="18" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1170,24 +1160,24 @@
         <v>16</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C18" s="1">
-        <v>60</v>
-      </c>
-      <c r="D18" s="1">
-        <v>1</v>
-      </c>
+        <v>100</v>
+      </c>
+      <c r="D18" s="1"/>
       <c r="E18" s="5" t="str">
         <f xml:space="preserve"> CONCATENATE(CEILING(Table1[[#This Row],[Current Part/Page]]/Table1[[#This Row],[Part/Page count]], 0.0001) * 100,"%")</f>
-        <v>1.67%</v>
-      </c>
-      <c r="F18" s="1"/>
+        <v>0%</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="G18" s="1"/>
-      <c r="H18" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="I18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="J18" s="1"/>
     </row>
     <row r="19" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1195,17 +1185,15 @@
         <v>17</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="C19" s="1">
-        <v>60</v>
-      </c>
-      <c r="D19" s="1">
-        <v>1</v>
-      </c>
+        <v>236</v>
+      </c>
+      <c r="D19" s="1"/>
       <c r="E19" s="5" t="str">
         <f xml:space="preserve"> CONCATENATE(CEILING(Table1[[#This Row],[Current Part/Page]]/Table1[[#This Row],[Part/Page count]], 0.0001) * 100,"%")</f>
-        <v>1.67%</v>
+        <v>0%</v>
       </c>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
@@ -1219,118 +1207,134 @@
       <c r="A20" s="9">
         <v>18</v>
       </c>
-      <c r="B20" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C20" s="1">
-        <v>52</v>
-      </c>
-      <c r="D20" s="1">
-        <v>42</v>
-      </c>
-      <c r="E20" s="5" t="str">
-        <f xml:space="preserve"> CONCATENATE(CEILING(Table1[[#This Row],[Current Part/Page]]/Table1[[#This Row],[Part/Page count]], 0.0001) * 100,"%")</f>
-        <v>80.77%</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G20" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="H20" s="3"/>
-      <c r="I20" s="1"/>
-      <c r="J20" s="1"/>
+      <c r="B20" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="C20" s="9">
+        <v>400</v>
+      </c>
+      <c r="D20" s="9">
+        <v>220</v>
+      </c>
+      <c r="E20" s="11" t="str">
+        <f xml:space="preserve"> CONCATENATE(CEILING(Table1[[#This Row],[Current Part/Page]]/Table1[[#This Row],[Part/Page count]], 0.0001) * 100,"%")</f>
+        <v>55%</v>
+      </c>
+      <c r="F20" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="G20" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="H20" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="I20" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="J20" s="9"/>
     </row>
     <row r="21" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="9">
         <v>19</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B21" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="C21" s="1">
-        <v>170</v>
-      </c>
-      <c r="D21" s="1"/>
-      <c r="E21" s="5" t="str">
+      <c r="C21" s="9">
+        <v>50</v>
+      </c>
+      <c r="D21" s="9"/>
+      <c r="E21" s="11" t="str">
         <f xml:space="preserve"> CONCATENATE(CEILING(Table1[[#This Row],[Current Part/Page]]/Table1[[#This Row],[Part/Page count]], 0.0001) * 100,"%")</f>
         <v>0%</v>
       </c>
-      <c r="F21" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G21" s="1"/>
-      <c r="H21" s="1"/>
-      <c r="I21" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="J21" s="1"/>
+      <c r="F21" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="G21" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="H21" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="I21" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="J21" s="9"/>
     </row>
     <row r="22" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="9">
         <v>20</v>
       </c>
-      <c r="B22" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C22" s="1">
-        <v>100</v>
-      </c>
-      <c r="D22" s="1"/>
-      <c r="E22" s="5" t="str">
+      <c r="B22" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="C22" s="9">
+        <v>1100</v>
+      </c>
+      <c r="D22" s="9"/>
+      <c r="E22" s="11" t="str">
         <f xml:space="preserve"> CONCATENATE(CEILING(Table1[[#This Row],[Current Part/Page]]/Table1[[#This Row],[Part/Page count]], 0.0001) * 100,"%")</f>
         <v>0%</v>
       </c>
-      <c r="F22" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G22" s="1"/>
-      <c r="H22" s="1"/>
-      <c r="I22" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="J22" s="1"/>
+      <c r="F22" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="G22" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="H22" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="I22" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="J22" s="9"/>
     </row>
     <row r="23" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="9">
         <v>21</v>
       </c>
-      <c r="B23" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C23" s="1">
-        <v>236</v>
-      </c>
-      <c r="D23" s="1"/>
-      <c r="E23" s="5" t="str">
+      <c r="B23" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="C23" s="9">
+        <v>600</v>
+      </c>
+      <c r="D23" s="9"/>
+      <c r="E23" s="11" t="str">
         <f xml:space="preserve"> CONCATENATE(CEILING(Table1[[#This Row],[Current Part/Page]]/Table1[[#This Row],[Part/Page count]], 0.0001) * 100,"%")</f>
         <v>0%</v>
       </c>
-      <c r="F23" s="1"/>
-      <c r="G23" s="1"/>
-      <c r="H23" s="1"/>
-      <c r="I23" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="J23" s="1"/>
+      <c r="F23" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="G23" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="H23" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="I23" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="J23" s="9"/>
     </row>
     <row r="24" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="9">
         <v>22</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C24" s="9">
-        <v>400</v>
-      </c>
-      <c r="D24" s="9">
-        <v>220</v>
-      </c>
+        <v>684</v>
+      </c>
+      <c r="D24" s="9"/>
       <c r="E24" s="11" t="str">
         <f xml:space="preserve"> CONCATENATE(CEILING(Table1[[#This Row],[Current Part/Page]]/Table1[[#This Row],[Part/Page count]], 0.0001) * 100,"%")</f>
-        <v>55%</v>
+        <v>0%</v>
       </c>
       <c r="F24" s="10" t="s">
         <v>16</v>
@@ -1351,10 +1355,10 @@
         <v>23</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C25" s="9">
-        <v>50</v>
+        <v>117</v>
       </c>
       <c r="D25" s="9"/>
       <c r="E25" s="11" t="str">
@@ -1380,10 +1384,10 @@
         <v>24</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C26" s="9">
-        <v>1100</v>
+        <v>1122</v>
       </c>
       <c r="D26" s="9"/>
       <c r="E26" s="11" t="str">
@@ -1409,10 +1413,10 @@
         <v>25</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C27" s="9">
-        <v>600</v>
+        <v>375</v>
       </c>
       <c r="D27" s="9"/>
       <c r="E27" s="11" t="str">
@@ -1441,12 +1445,14 @@
         <v>42</v>
       </c>
       <c r="C28" s="9">
-        <v>684</v>
-      </c>
-      <c r="D28" s="9"/>
+        <v>550</v>
+      </c>
+      <c r="D28" s="9">
+        <v>115</v>
+      </c>
       <c r="E28" s="11" t="str">
         <f xml:space="preserve"> CONCATENATE(CEILING(Table1[[#This Row],[Current Part/Page]]/Table1[[#This Row],[Part/Page count]], 0.0001) * 100,"%")</f>
-        <v>0%</v>
+        <v>20.91%</v>
       </c>
       <c r="F28" s="10" t="s">
         <v>16</v>
@@ -1470,12 +1476,14 @@
         <v>43</v>
       </c>
       <c r="C29" s="9">
-        <v>117</v>
-      </c>
-      <c r="D29" s="9"/>
+        <v>504</v>
+      </c>
+      <c r="D29" s="9">
+        <v>210</v>
+      </c>
       <c r="E29" s="11" t="str">
         <f xml:space="preserve"> CONCATENATE(CEILING(Table1[[#This Row],[Current Part/Page]]/Table1[[#This Row],[Part/Page count]], 0.0001) * 100,"%")</f>
-        <v>0%</v>
+        <v>41.67%</v>
       </c>
       <c r="F29" s="10" t="s">
         <v>16</v>
@@ -1499,7 +1507,7 @@
         <v>44</v>
       </c>
       <c r="C30" s="9">
-        <v>1122</v>
+        <v>1321</v>
       </c>
       <c r="D30" s="9"/>
       <c r="E30" s="11" t="str">
@@ -1528,7 +1536,7 @@
         <v>45</v>
       </c>
       <c r="C31" s="9">
-        <v>375</v>
+        <v>400</v>
       </c>
       <c r="D31" s="9"/>
       <c r="E31" s="11" t="str">
@@ -1554,17 +1562,15 @@
         <v>30</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="C32" s="9">
-        <v>550</v>
-      </c>
-      <c r="D32" s="9">
-        <v>115</v>
-      </c>
+        <v>1100</v>
+      </c>
+      <c r="D32" s="9"/>
       <c r="E32" s="11" t="str">
         <f xml:space="preserve"> CONCATENATE(CEILING(Table1[[#This Row],[Current Part/Page]]/Table1[[#This Row],[Part/Page count]], 0.0001) * 100,"%")</f>
-        <v>20.91%</v>
+        <v>0%</v>
       </c>
       <c r="F32" s="10" t="s">
         <v>16</v>
@@ -1585,138 +1591,140 @@
         <v>31</v>
       </c>
       <c r="B33" s="9" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C33" s="9">
-        <v>504</v>
+        <v>97</v>
       </c>
       <c r="D33" s="9">
-        <v>210</v>
+        <v>79</v>
       </c>
       <c r="E33" s="11" t="str">
         <f xml:space="preserve"> CONCATENATE(CEILING(Table1[[#This Row],[Current Part/Page]]/Table1[[#This Row],[Part/Page count]], 0.0001) * 100,"%")</f>
-        <v>41.67%</v>
-      </c>
-      <c r="F33" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="G33" s="10" t="s">
-        <v>16</v>
-      </c>
+        <v>81.45%</v>
+      </c>
+      <c r="F33" s="10"/>
+      <c r="G33" s="10"/>
       <c r="H33" s="10" t="s">
         <v>16</v>
       </c>
       <c r="I33" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="J33" s="9"/>
+      <c r="J33" s="9" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="34" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="9">
         <v>32</v>
       </c>
       <c r="B34" s="9" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="C34" s="9">
-        <v>1321</v>
-      </c>
-      <c r="D34" s="9"/>
+        <v>170</v>
+      </c>
+      <c r="D34" s="9">
+        <v>170</v>
+      </c>
       <c r="E34" s="11" t="str">
         <f xml:space="preserve"> CONCATENATE(CEILING(Table1[[#This Row],[Current Part/Page]]/Table1[[#This Row],[Part/Page count]], 0.0001) * 100,"%")</f>
-        <v>0%</v>
+        <v>100%</v>
       </c>
       <c r="F34" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="G34" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="H34" s="10" t="s">
-        <v>16</v>
-      </c>
+      <c r="G34" s="10"/>
+      <c r="H34" s="10"/>
       <c r="I34" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="J34" s="9"/>
+      <c r="J34" s="9" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="35" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="9">
         <v>33</v>
       </c>
       <c r="B35" s="9" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="C35" s="9">
-        <v>400</v>
-      </c>
-      <c r="D35" s="9"/>
+        <v>115</v>
+      </c>
+      <c r="D35" s="9">
+        <v>40</v>
+      </c>
       <c r="E35" s="11" t="str">
         <f xml:space="preserve"> CONCATENATE(CEILING(Table1[[#This Row],[Current Part/Page]]/Table1[[#This Row],[Part/Page count]], 0.0001) * 100,"%")</f>
-        <v>0%</v>
-      </c>
-      <c r="F35" s="10" t="s">
-        <v>16</v>
-      </c>
+        <v>34.79%</v>
+      </c>
+      <c r="F35" s="10"/>
       <c r="G35" s="10" t="s">
         <v>16</v>
       </c>
       <c r="H35" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="I35" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="J35" s="9"/>
+      <c r="I35" s="10"/>
+      <c r="J35" s="9" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="36" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="9">
         <v>34</v>
       </c>
       <c r="B36" s="9" t="s">
-        <v>41</v>
+        <v>53</v>
       </c>
       <c r="C36" s="9">
-        <v>1100</v>
-      </c>
-      <c r="D36" s="9"/>
+        <v>528</v>
+      </c>
+      <c r="D36" s="9">
+        <v>70</v>
+      </c>
       <c r="E36" s="11" t="str">
         <f xml:space="preserve"> CONCATENATE(CEILING(Table1[[#This Row],[Current Part/Page]]/Table1[[#This Row],[Part/Page count]], 0.0001) * 100,"%")</f>
-        <v>0%</v>
+        <v>13.26%</v>
       </c>
       <c r="F36" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="G36" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="H36" s="10" t="s">
-        <v>16</v>
-      </c>
+      <c r="G36" s="10"/>
+      <c r="H36" s="10"/>
       <c r="I36" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="J36" s="9"/>
+      <c r="J36" s="9" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="37" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="9">
         <v>35</v>
       </c>
       <c r="B37" s="9" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="C37" s="9">
-        <v>97</v>
+        <v>30</v>
       </c>
       <c r="D37" s="9">
-        <v>79</v>
+        <v>9</v>
       </c>
       <c r="E37" s="11" t="str">
         <f xml:space="preserve"> CONCATENATE(CEILING(Table1[[#This Row],[Current Part/Page]]/Table1[[#This Row],[Part/Page count]], 0.0001) * 100,"%")</f>
-        <v>81.45%</v>
-      </c>
-      <c r="F37" s="10"/>
-      <c r="G37" s="10"/>
+        <v>30%</v>
+      </c>
+      <c r="F37" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="G37" s="10" t="s">
+        <v>16</v>
+      </c>
       <c r="H37" s="10" t="s">
         <v>16</v>
       </c>
@@ -1724,7 +1732,7 @@
         <v>16</v>
       </c>
       <c r="J37" s="9" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
     </row>
     <row r="38" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1732,57 +1740,59 @@
         <v>36</v>
       </c>
       <c r="B38" s="9" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C38" s="9">
-        <v>170</v>
+        <v>120</v>
       </c>
       <c r="D38" s="9">
-        <v>108</v>
+        <v>15</v>
       </c>
       <c r="E38" s="11" t="str">
         <f xml:space="preserve"> CONCATENATE(CEILING(Table1[[#This Row],[Current Part/Page]]/Table1[[#This Row],[Part/Page count]], 0.0001) * 100,"%")</f>
-        <v>63.53%</v>
-      </c>
-      <c r="F38" s="10" t="s">
-        <v>16</v>
-      </c>
+        <v>12.5%</v>
+      </c>
+      <c r="F38" s="10"/>
       <c r="G38" s="10"/>
-      <c r="H38" s="10"/>
+      <c r="H38" s="10" t="s">
+        <v>16</v>
+      </c>
       <c r="I38" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="J38" s="9" t="s">
-        <v>56</v>
-      </c>
+      <c r="J38" s="9"/>
     </row>
     <row r="39" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="9">
         <v>37</v>
       </c>
       <c r="B39" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="C39" s="9">
+        <v>80</v>
+      </c>
+      <c r="D39" s="9">
+        <v>29</v>
+      </c>
+      <c r="E39" s="11" t="str">
+        <f xml:space="preserve"> CONCATENATE(CEILING(Table1[[#This Row],[Current Part/Page]]/Table1[[#This Row],[Part/Page count]], 0.0001) * 100,"%")</f>
+        <v>36.25%</v>
+      </c>
+      <c r="F39" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="G39" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="H39" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="I39" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="J39" s="9" t="s">
         <v>58</v>
-      </c>
-      <c r="C39" s="9">
-        <v>115</v>
-      </c>
-      <c r="D39" s="9">
-        <v>28</v>
-      </c>
-      <c r="E39" s="11" t="str">
-        <f xml:space="preserve"> CONCATENATE(CEILING(Table1[[#This Row],[Current Part/Page]]/Table1[[#This Row],[Part/Page count]], 0.0001) * 100,"%")</f>
-        <v>24.35%</v>
-      </c>
-      <c r="F39" s="10"/>
-      <c r="G39" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="H39" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="I39" s="10"/>
-      <c r="J39" s="9" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="40" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1790,46 +1800,46 @@
         <v>38</v>
       </c>
       <c r="B40" s="9" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="C40" s="9">
-        <v>528</v>
+        <v>190</v>
       </c>
       <c r="D40" s="9">
-        <v>70</v>
+        <v>35</v>
       </c>
       <c r="E40" s="11" t="str">
         <f xml:space="preserve"> CONCATENATE(CEILING(Table1[[#This Row],[Current Part/Page]]/Table1[[#This Row],[Part/Page count]], 0.0001) * 100,"%")</f>
-        <v>13.26%</v>
+        <v>18.43%</v>
       </c>
       <c r="F40" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="G40" s="10"/>
-      <c r="H40" s="10"/>
+      <c r="G40" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="H40" s="10" t="s">
+        <v>16</v>
+      </c>
       <c r="I40" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="J40" s="9" t="s">
-        <v>63</v>
-      </c>
+      <c r="J40" s="9"/>
     </row>
     <row r="41" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="9">
         <v>39</v>
       </c>
       <c r="B41" s="9" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C41" s="9">
-        <v>30</v>
-      </c>
-      <c r="D41" s="9">
-        <v>4</v>
-      </c>
+        <v>186</v>
+      </c>
+      <c r="D41" s="9"/>
       <c r="E41" s="11" t="str">
         <f xml:space="preserve"> CONCATENATE(CEILING(Table1[[#This Row],[Current Part/Page]]/Table1[[#This Row],[Part/Page count]], 0.0001) * 100,"%")</f>
-        <v>13.34%</v>
+        <v>0%</v>
       </c>
       <c r="F41" s="10" t="s">
         <v>16</v>
@@ -1843,29 +1853,31 @@
       <c r="I41" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="J41" s="9" t="s">
-        <v>63</v>
-      </c>
+      <c r="J41" s="9"/>
     </row>
     <row r="42" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="9">
         <v>40</v>
       </c>
       <c r="B42" s="9" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C42" s="9">
-        <v>120</v>
+        <v>130</v>
       </c>
       <c r="D42" s="9">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E42" s="11" t="str">
         <f xml:space="preserve"> CONCATENATE(CEILING(Table1[[#This Row],[Current Part/Page]]/Table1[[#This Row],[Part/Page count]], 0.0001) * 100,"%")</f>
-        <v>12.5%</v>
-      </c>
-      <c r="F42" s="10"/>
-      <c r="G42" s="10"/>
+        <v>10%</v>
+      </c>
+      <c r="F42" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="G42" s="10" t="s">
+        <v>16</v>
+      </c>
       <c r="H42" s="10" t="s">
         <v>16</v>
       </c>
@@ -1879,148 +1891,30 @@
         <v>41</v>
       </c>
       <c r="B43" s="9" t="s">
-        <v>61</v>
+        <v>28</v>
       </c>
       <c r="C43" s="9">
-        <v>80</v>
-      </c>
-      <c r="D43" s="9">
-        <v>29</v>
-      </c>
+        <v>200</v>
+      </c>
+      <c r="D43" s="9"/>
       <c r="E43" s="11" t="str">
         <f xml:space="preserve"> CONCATENATE(CEILING(Table1[[#This Row],[Current Part/Page]]/Table1[[#This Row],[Part/Page count]], 0.0001) * 100,"%")</f>
-        <v>36.25%</v>
-      </c>
-      <c r="F43" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="G43" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="H43" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="I43" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="J43" s="9" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="9">
-        <v>42</v>
-      </c>
-      <c r="B44" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="C44" s="9">
-        <v>190</v>
-      </c>
-      <c r="D44" s="9">
-        <v>10</v>
-      </c>
-      <c r="E44" s="11" t="str">
-        <f xml:space="preserve"> CONCATENATE(CEILING(Table1[[#This Row],[Current Part/Page]]/Table1[[#This Row],[Part/Page count]], 0.0001) * 100,"%")</f>
-        <v>5.27%</v>
-      </c>
-      <c r="F44" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="G44" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="H44" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="I44" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="J44" s="9"/>
-    </row>
-    <row r="45" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="9">
-        <v>43</v>
-      </c>
-      <c r="B45" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="C45" s="9">
-        <v>186</v>
-      </c>
-      <c r="D45" s="9"/>
-      <c r="E45" s="11" t="str">
-        <f xml:space="preserve"> CONCATENATE(CEILING(Table1[[#This Row],[Current Part/Page]]/Table1[[#This Row],[Part/Page count]], 0.0001) * 100,"%")</f>
         <v>0%</v>
       </c>
-      <c r="F45" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="G45" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="H45" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="I45" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="J45" s="9"/>
-    </row>
-    <row r="46" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="9">
-        <v>44</v>
-      </c>
-      <c r="B46" s="9" t="s">
-        <v>66</v>
-      </c>
-      <c r="C46" s="9">
-        <v>130</v>
-      </c>
-      <c r="D46" s="9"/>
-      <c r="E46" s="11" t="str">
-        <f xml:space="preserve"> CONCATENATE(CEILING(Table1[[#This Row],[Current Part/Page]]/Table1[[#This Row],[Part/Page count]], 0.0001) * 100,"%")</f>
-        <v>0%</v>
-      </c>
-      <c r="F46" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="G46" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="H46" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="I46" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="J46" s="9"/>
-    </row>
-    <row r="47" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="9">
-        <v>42</v>
-      </c>
-      <c r="B47" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="C47" s="9">
-        <v>200</v>
-      </c>
-      <c r="D47" s="9"/>
-      <c r="E47" s="11" t="str">
-        <f xml:space="preserve"> CONCATENATE(CEILING(Table1[[#This Row],[Current Part/Page]]/Table1[[#This Row],[Part/Page count]], 0.0001) * 100,"%")</f>
-        <v>0%</v>
-      </c>
-      <c r="F47" s="9"/>
-      <c r="G47" s="9"/>
-      <c r="H47" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="I47" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="J47" s="9"/>
-    </row>
+      <c r="F43" s="9"/>
+      <c r="G43" s="9"/>
+      <c r="H43" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="I43" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="J43" s="9"/>
+    </row>
+    <row r="44" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="45" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="46" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="47" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="48" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="1">
@@ -2038,8 +1932,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J56"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="C42" sqref="C42"/>
+    <sheetView topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="C53" sqref="C53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2070,10 +1964,10 @@
         <v>15</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="H1" s="14" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="I1" s="14"/>
       <c r="J1" s="14"/>
@@ -2755,13 +2649,17 @@
       <c r="A51" s="1">
         <v>50</v>
       </c>
-      <c r="B51" s="8"/>
-      <c r="C51" s="8"/>
+      <c r="B51" s="8">
+        <v>23</v>
+      </c>
+      <c r="C51" s="8">
+        <v>22</v>
+      </c>
       <c r="D51" s="8"/>
       <c r="E51" s="8"/>
       <c r="F51" s="8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>45</v>
       </c>
     </row>
     <row r="52" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2818,15 +2716,15 @@
     </row>
     <row r="56" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B56" s="8">
         <f xml:space="preserve"> AVERAGE(B2:B55)</f>
-        <v>20.666666666666668</v>
+        <v>21</v>
       </c>
       <c r="C56" s="8">
         <f t="shared" ref="C56:E56" si="1" xml:space="preserve"> AVERAGE(C2:C55)</f>
-        <v>24.25</v>
+        <v>24</v>
       </c>
       <c r="D56" s="8">
         <f t="shared" si="1"/>
@@ -2838,7 +2736,7 @@
       </c>
       <c r="F56" s="8">
         <f xml:space="preserve"> SUM(B56, C56, D56, E56)</f>
-        <v>84.916666666666671</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Change the txt file into a docx one
</commit_message>
<xml_diff>
--- a/TOEFL/Progress.xlsx
+++ b/TOEFL/Progress.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="16380" yWindow="0" windowWidth="16980" windowHeight="8205"/>
+    <workbookView xWindow="17550" yWindow="0" windowWidth="16980" windowHeight="8205"/>
   </bookViews>
   <sheets>
     <sheet name="Progress" sheetId="1" r:id="rId1"/>
@@ -715,8 +715,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D38" sqref="D38"/>
+    <sheetView tabSelected="1" topLeftCell="A20" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1597,11 +1597,11 @@
         <v>97</v>
       </c>
       <c r="D33" s="9">
-        <v>79</v>
+        <v>97</v>
       </c>
       <c r="E33" s="11" t="str">
         <f xml:space="preserve"> CONCATENATE(CEILING(Table1[[#This Row],[Current Part/Page]]/Table1[[#This Row],[Part/Page count]], 0.0001) * 100,"%")</f>
-        <v>81.45%</v>
+        <v>100%</v>
       </c>
       <c r="F33" s="10"/>
       <c r="G33" s="10"/>
@@ -1713,11 +1713,11 @@
         <v>30</v>
       </c>
       <c r="D37" s="9">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E37" s="11" t="str">
         <f xml:space="preserve"> CONCATENATE(CEILING(Table1[[#This Row],[Current Part/Page]]/Table1[[#This Row],[Part/Page count]], 0.0001) * 100,"%")</f>
-        <v>30%</v>
+        <v>33.34%</v>
       </c>
       <c r="F37" s="10" t="s">
         <v>16</v>

</xml_diff>

<commit_message>
Update Progress.xlsx, add 2 Books (Writing Power, The American Accent) and 1 Podcast (BBC - 6 Minute English 2019)
</commit_message>
<xml_diff>
--- a/TOEFL/Progress.xlsx
+++ b/TOEFL/Progress.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="19890" yWindow="0" windowWidth="16980" windowHeight="8205"/>
+    <workbookView xWindow="20895" yWindow="0" windowWidth="16980" windowHeight="8205"/>
   </bookViews>
   <sheets>
     <sheet name="Progress" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="61">
   <si>
     <t>Book/CD Name</t>
   </si>
@@ -191,6 +191,18 @@
   </si>
   <si>
     <t>Check your vocabulary for TOEFL</t>
+  </si>
+  <si>
+    <t>Writing Power - Kaplan</t>
+  </si>
+  <si>
+    <t>BBC Podcasts - 6MinEnglish - 2017</t>
+  </si>
+  <si>
+    <t>BBC Podcasts - 6MinEnglish - 2019</t>
+  </si>
+  <si>
+    <t>The American Accent</t>
   </si>
 </sst>
 </file>
@@ -392,8 +404,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A2:J37" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18">
-  <autoFilter ref="A2:J37"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A2:J41" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18">
+  <autoFilter ref="A2:J41"/>
   <tableColumns count="10">
     <tableColumn id="1" name="No." dataDxfId="17"/>
     <tableColumn id="2" name="Book/CD Name" dataDxfId="16"/>
@@ -692,10 +704,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J42"/>
+  <dimension ref="A1:J44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -972,156 +984,143 @@
       <c r="J10" s="1"/>
     </row>
     <row r="11" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="8">
-        <v>9</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C11" s="1">
+      <c r="A11" s="8"/>
+      <c r="B11" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="C11" s="8">
         <v>52</v>
       </c>
-      <c r="D11" s="1">
+      <c r="D11" s="8">
         <v>52</v>
       </c>
-      <c r="E11" s="4" t="str">
+      <c r="E11" s="10" t="str">
         <f xml:space="preserve"> CONCATENATE(CEILING(Table1[[#This Row],[Current Part/Page]]/Table1[[#This Row],[Part/Page count]], 0.0001) * 100,"%")</f>
         <v>100%</v>
       </c>
-      <c r="F11" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H11" s="2"/>
-      <c r="I11" s="1"/>
-      <c r="J11" s="1"/>
+      <c r="F11" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="G11" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="H11" s="8"/>
+      <c r="I11" s="8"/>
+      <c r="J11" s="8"/>
     </row>
     <row r="12" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="8">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>24</v>
+        <v>43</v>
       </c>
       <c r="C12" s="1">
-        <v>170</v>
+        <v>52</v>
       </c>
       <c r="D12" s="1">
-        <v>30</v>
+        <v>52</v>
       </c>
       <c r="E12" s="4" t="str">
         <f xml:space="preserve"> CONCATENATE(CEILING(Table1[[#This Row],[Current Part/Page]]/Table1[[#This Row],[Part/Page count]], 0.0001) * 100,"%")</f>
-        <v>17.65%</v>
+        <v>100%</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
-      <c r="I12" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="J12" s="1"/>
+      <c r="G12" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H12" s="8"/>
+      <c r="I12" s="8"/>
+      <c r="J12" s="8"/>
     </row>
     <row r="13" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="8">
-        <v>11</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C13" s="1">
-        <v>236</v>
-      </c>
-      <c r="D13" s="1"/>
-      <c r="E13" s="4" t="str">
-        <f xml:space="preserve"> CONCATENATE(CEILING(Table1[[#This Row],[Current Part/Page]]/Table1[[#This Row],[Part/Page count]], 0.0001) * 100,"%")</f>
-        <v>0%</v>
-      </c>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
-      <c r="I13" s="1" t="s">
-        <v>15</v>
-      </c>
+      <c r="A13" s="8"/>
+      <c r="B13" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="C13" s="8">
+        <v>52</v>
+      </c>
+      <c r="D13" s="8"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="G13" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="H13" s="2"/>
+      <c r="I13" s="1"/>
       <c r="J13" s="1"/>
     </row>
     <row r="14" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="8">
-        <v>12</v>
-      </c>
-      <c r="B14" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="C14" s="8">
-        <v>400</v>
-      </c>
-      <c r="D14" s="8">
-        <v>400</v>
-      </c>
-      <c r="E14" s="10" t="str">
-        <f xml:space="preserve"> CONCATENATE(CEILING(Table1[[#This Row],[Current Part/Page]]/Table1[[#This Row],[Part/Page count]], 0.0001) * 100,"%")</f>
-        <v>100%</v>
-      </c>
-      <c r="F14" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="G14" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="H14" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="I14" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="J14" s="8"/>
+        <v>10</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" s="1">
+        <v>170</v>
+      </c>
+      <c r="D14" s="1">
+        <v>30</v>
+      </c>
+      <c r="E14" s="4" t="str">
+        <f xml:space="preserve"> CONCATENATE(CEILING(Table1[[#This Row],[Current Part/Page]]/Table1[[#This Row],[Part/Page count]], 0.0001) * 100,"%")</f>
+        <v>17.65%</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J14" s="1"/>
     </row>
     <row r="15" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="8">
-        <v>13</v>
-      </c>
-      <c r="B15" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="C15" s="8">
-        <v>50</v>
-      </c>
-      <c r="D15" s="8"/>
-      <c r="E15" s="10" t="str">
+        <v>11</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" s="1">
+        <v>236</v>
+      </c>
+      <c r="D15" s="1"/>
+      <c r="E15" s="4" t="str">
         <f xml:space="preserve"> CONCATENATE(CEILING(Table1[[#This Row],[Current Part/Page]]/Table1[[#This Row],[Part/Page count]], 0.0001) * 100,"%")</f>
         <v>0%</v>
       </c>
-      <c r="F15" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="G15" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="H15" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="I15" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="J15" s="8"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J15" s="1"/>
     </row>
     <row r="16" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="8">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C16" s="8">
-        <v>1100</v>
-      </c>
-      <c r="D16" s="8"/>
+        <v>400</v>
+      </c>
+      <c r="D16" s="8">
+        <v>400</v>
+      </c>
       <c r="E16" s="10" t="str">
         <f xml:space="preserve"> CONCATENATE(CEILING(Table1[[#This Row],[Current Part/Page]]/Table1[[#This Row],[Part/Page count]], 0.0001) * 100,"%")</f>
-        <v>0%</v>
+        <v>100%</v>
       </c>
       <c r="F16" s="9" t="s">
         <v>15</v>
@@ -1139,13 +1138,13 @@
     </row>
     <row r="17" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="8">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C17" s="8">
-        <v>600</v>
+        <v>50</v>
       </c>
       <c r="D17" s="8"/>
       <c r="E17" s="10" t="str">
@@ -1168,13 +1167,13 @@
     </row>
     <row r="18" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="8">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C18" s="8">
-        <v>684</v>
+        <v>1100</v>
       </c>
       <c r="D18" s="8"/>
       <c r="E18" s="10" t="str">
@@ -1197,13 +1196,13 @@
     </row>
     <row r="19" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="8">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C19" s="8">
-        <v>117</v>
+        <v>600</v>
       </c>
       <c r="D19" s="8"/>
       <c r="E19" s="10" t="str">
@@ -1226,13 +1225,13 @@
     </row>
     <row r="20" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="8">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C20" s="8">
-        <v>1122</v>
+        <v>684</v>
       </c>
       <c r="D20" s="8"/>
       <c r="E20" s="10" t="str">
@@ -1255,13 +1254,13 @@
     </row>
     <row r="21" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="8">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C21" s="8">
-        <v>375</v>
+        <v>117</v>
       </c>
       <c r="D21" s="8"/>
       <c r="E21" s="10" t="str">
@@ -1284,20 +1283,18 @@
     </row>
     <row r="22" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="8">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C22" s="8">
-        <v>550</v>
-      </c>
-      <c r="D22" s="8">
-        <v>550</v>
-      </c>
+        <v>1122</v>
+      </c>
+      <c r="D22" s="8"/>
       <c r="E22" s="10" t="str">
         <f xml:space="preserve"> CONCATENATE(CEILING(Table1[[#This Row],[Current Part/Page]]/Table1[[#This Row],[Part/Page count]], 0.0001) * 100,"%")</f>
-        <v>100%</v>
+        <v>0%</v>
       </c>
       <c r="F22" s="9" t="s">
         <v>15</v>
@@ -1315,20 +1312,18 @@
     </row>
     <row r="23" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="8">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C23" s="8">
-        <v>504</v>
-      </c>
-      <c r="D23" s="8">
-        <v>504</v>
-      </c>
+        <v>375</v>
+      </c>
+      <c r="D23" s="8"/>
       <c r="E23" s="10" t="str">
         <f xml:space="preserve"> CONCATENATE(CEILING(Table1[[#This Row],[Current Part/Page]]/Table1[[#This Row],[Part/Page count]], 0.0001) * 100,"%")</f>
-        <v>100%</v>
+        <v>0%</v>
       </c>
       <c r="F23" s="9" t="s">
         <v>15</v>
@@ -1346,18 +1341,20 @@
     </row>
     <row r="24" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="8">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C24" s="8">
-        <v>1321</v>
-      </c>
-      <c r="D24" s="8"/>
+        <v>550</v>
+      </c>
+      <c r="D24" s="8">
+        <v>550</v>
+      </c>
       <c r="E24" s="10" t="str">
         <f xml:space="preserve"> CONCATENATE(CEILING(Table1[[#This Row],[Current Part/Page]]/Table1[[#This Row],[Part/Page count]], 0.0001) * 100,"%")</f>
-        <v>0%</v>
+        <v>100%</v>
       </c>
       <c r="F24" s="9" t="s">
         <v>15</v>
@@ -1375,18 +1372,20 @@
     </row>
     <row r="25" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="8">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C25" s="8">
-        <v>400</v>
-      </c>
-      <c r="D25" s="8"/>
+        <v>504</v>
+      </c>
+      <c r="D25" s="8">
+        <v>504</v>
+      </c>
       <c r="E25" s="10" t="str">
         <f xml:space="preserve"> CONCATENATE(CEILING(Table1[[#This Row],[Current Part/Page]]/Table1[[#This Row],[Part/Page count]], 0.0001) * 100,"%")</f>
-        <v>0%</v>
+        <v>100%</v>
       </c>
       <c r="F25" s="9" t="s">
         <v>15</v>
@@ -1404,13 +1403,13 @@
     </row>
     <row r="26" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="8">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="C26" s="8">
-        <v>1100</v>
+        <v>1321</v>
       </c>
       <c r="D26" s="8"/>
       <c r="E26" s="10" t="str">
@@ -1433,107 +1432,107 @@
     </row>
     <row r="27" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="8">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C27" s="8">
-        <v>97</v>
-      </c>
-      <c r="D27" s="8">
-        <v>97</v>
-      </c>
+        <v>400</v>
+      </c>
+      <c r="D27" s="8"/>
       <c r="E27" s="10" t="str">
         <f xml:space="preserve"> CONCATENATE(CEILING(Table1[[#This Row],[Current Part/Page]]/Table1[[#This Row],[Part/Page count]], 0.0001) * 100,"%")</f>
-        <v>100%</v>
-      </c>
-      <c r="F27" s="9"/>
-      <c r="G27" s="9"/>
+        <v>0%</v>
+      </c>
+      <c r="F27" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G27" s="9" t="s">
+        <v>15</v>
+      </c>
       <c r="H27" s="9" t="s">
         <v>15</v>
       </c>
       <c r="I27" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="J27" s="8" t="s">
-        <v>44</v>
-      </c>
+      <c r="J27" s="8"/>
     </row>
     <row r="28" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="8">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C28" s="8">
-        <v>170</v>
-      </c>
-      <c r="D28" s="8">
-        <v>170</v>
-      </c>
+        <v>1100</v>
+      </c>
+      <c r="D28" s="8"/>
       <c r="E28" s="10" t="str">
         <f xml:space="preserve"> CONCATENATE(CEILING(Table1[[#This Row],[Current Part/Page]]/Table1[[#This Row],[Part/Page count]], 0.0001) * 100,"%")</f>
-        <v>100%</v>
+        <v>0%</v>
       </c>
       <c r="F28" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="G28" s="9"/>
-      <c r="H28" s="9"/>
+      <c r="G28" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="H28" s="9" t="s">
+        <v>15</v>
+      </c>
       <c r="I28" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="J28" s="8" t="s">
-        <v>46</v>
-      </c>
+      <c r="J28" s="8"/>
     </row>
     <row r="29" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="8">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="C29" s="8">
-        <v>115</v>
+        <v>97</v>
       </c>
       <c r="D29" s="8">
-        <v>40</v>
+        <v>97</v>
       </c>
       <c r="E29" s="10" t="str">
         <f xml:space="preserve"> CONCATENATE(CEILING(Table1[[#This Row],[Current Part/Page]]/Table1[[#This Row],[Part/Page count]], 0.0001) * 100,"%")</f>
-        <v>34.79%</v>
+        <v>100%</v>
       </c>
       <c r="F29" s="9"/>
-      <c r="G29" s="9" t="s">
-        <v>15</v>
-      </c>
+      <c r="G29" s="9"/>
       <c r="H29" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="I29" s="9"/>
+      <c r="I29" s="9" t="s">
+        <v>15</v>
+      </c>
       <c r="J29" s="8" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
     </row>
     <row r="30" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="8">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C30" s="8">
-        <v>528</v>
+        <v>170</v>
       </c>
       <c r="D30" s="8">
-        <v>70</v>
+        <v>170</v>
       </c>
       <c r="E30" s="10" t="str">
         <f xml:space="preserve"> CONCATENATE(CEILING(Table1[[#This Row],[Current Part/Page]]/Table1[[#This Row],[Part/Page count]], 0.0001) * 100,"%")</f>
-        <v>13.26%</v>
+        <v>100%</v>
       </c>
       <c r="F30" s="9" t="s">
         <v>15</v>
@@ -1544,85 +1543,83 @@
         <v>15</v>
       </c>
       <c r="J30" s="8" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
     </row>
     <row r="31" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="8">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C31" s="8">
-        <v>30</v>
+        <v>115</v>
       </c>
       <c r="D31" s="8">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="E31" s="10" t="str">
         <f xml:space="preserve"> CONCATENATE(CEILING(Table1[[#This Row],[Current Part/Page]]/Table1[[#This Row],[Part/Page count]], 0.0001) * 100,"%")</f>
-        <v>33.34%</v>
-      </c>
-      <c r="F31" s="9" t="s">
-        <v>15</v>
-      </c>
+        <v>34.79%</v>
+      </c>
+      <c r="F31" s="9"/>
       <c r="G31" s="9" t="s">
         <v>15</v>
       </c>
       <c r="H31" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="I31" s="9" t="s">
-        <v>15</v>
-      </c>
+      <c r="I31" s="9"/>
       <c r="J31" s="8" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="32" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="8">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C32" s="8">
-        <v>60</v>
+        <v>528</v>
       </c>
       <c r="D32" s="8">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="E32" s="10" t="str">
         <f xml:space="preserve"> CONCATENATE(CEILING(Table1[[#This Row],[Current Part/Page]]/Table1[[#This Row],[Part/Page count]], 0.0001) * 100,"%")</f>
-        <v>100%</v>
-      </c>
-      <c r="F32" s="9"/>
+        <v>13.26%</v>
+      </c>
+      <c r="F32" s="9" t="s">
+        <v>15</v>
+      </c>
       <c r="G32" s="9"/>
-      <c r="H32" s="9" t="s">
-        <v>15</v>
-      </c>
+      <c r="H32" s="9"/>
       <c r="I32" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="J32" s="8"/>
+      <c r="J32" s="8" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="33" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="8">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C33" s="8">
-        <v>80</v>
+        <v>30</v>
       </c>
       <c r="D33" s="8">
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="E33" s="10" t="str">
         <f xml:space="preserve"> CONCATENATE(CEILING(Table1[[#This Row],[Current Part/Page]]/Table1[[#This Row],[Part/Page count]], 0.0001) * 100,"%")</f>
-        <v>36.25%</v>
+        <v>33.34%</v>
       </c>
       <c r="F33" s="9" t="s">
         <v>15</v>
@@ -1637,32 +1634,28 @@
         <v>15</v>
       </c>
       <c r="J33" s="8" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="34" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="8">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C34" s="8">
-        <v>190</v>
+        <v>60</v>
       </c>
       <c r="D34" s="8">
-        <v>35</v>
+        <v>60</v>
       </c>
       <c r="E34" s="10" t="str">
         <f xml:space="preserve"> CONCATENATE(CEILING(Table1[[#This Row],[Current Part/Page]]/Table1[[#This Row],[Part/Page count]], 0.0001) * 100,"%")</f>
-        <v>18.43%</v>
-      </c>
-      <c r="F34" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="G34" s="9" t="s">
-        <v>15</v>
-      </c>
+        <v>100%</v>
+      </c>
+      <c r="F34" s="9"/>
+      <c r="G34" s="9"/>
       <c r="H34" s="9" t="s">
         <v>15</v>
       </c>
@@ -1673,18 +1666,20 @@
     </row>
     <row r="35" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="8">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C35" s="8">
-        <v>186</v>
-      </c>
-      <c r="D35" s="8"/>
+        <v>80</v>
+      </c>
+      <c r="D35" s="8">
+        <v>29</v>
+      </c>
       <c r="E35" s="10" t="str">
         <f xml:space="preserve"> CONCATENATE(CEILING(Table1[[#This Row],[Current Part/Page]]/Table1[[#This Row],[Part/Page count]], 0.0001) * 100,"%")</f>
-        <v>0%</v>
+        <v>36.25%</v>
       </c>
       <c r="F35" s="9" t="s">
         <v>15</v>
@@ -1698,24 +1693,26 @@
       <c r="I35" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="J35" s="8"/>
+      <c r="J35" s="8" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="36" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="8">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C36" s="8">
-        <v>130</v>
+        <v>190</v>
       </c>
       <c r="D36" s="8">
-        <v>13</v>
+        <v>35</v>
       </c>
       <c r="E36" s="10" t="str">
         <f xml:space="preserve"> CONCATENATE(CEILING(Table1[[#This Row],[Current Part/Page]]/Table1[[#This Row],[Part/Page count]], 0.0001) * 100,"%")</f>
-        <v>10%</v>
+        <v>18.43%</v>
       </c>
       <c r="F36" s="9" t="s">
         <v>15</v>
@@ -1733,40 +1730,159 @@
     </row>
     <row r="37" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="8">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B37" s="8" t="s">
-        <v>23</v>
+        <v>55</v>
       </c>
       <c r="C37" s="8">
-        <v>200</v>
+        <v>186</v>
       </c>
       <c r="D37" s="8"/>
       <c r="E37" s="10" t="str">
         <f xml:space="preserve"> CONCATENATE(CEILING(Table1[[#This Row],[Current Part/Page]]/Table1[[#This Row],[Part/Page count]], 0.0001) * 100,"%")</f>
         <v>0%</v>
       </c>
-      <c r="F37" s="8"/>
-      <c r="G37" s="8"/>
-      <c r="H37" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="I37" s="8" t="s">
+      <c r="F37" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G37" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="H37" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="I37" s="9" t="s">
         <v>15</v>
       </c>
       <c r="J37" s="8"/>
     </row>
-    <row r="38" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="39" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="40" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="41" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="42" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="38" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="8">
+        <v>34</v>
+      </c>
+      <c r="B38" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="C38" s="8">
+        <v>130</v>
+      </c>
+      <c r="D38" s="8">
+        <v>13</v>
+      </c>
+      <c r="E38" s="10" t="str">
+        <f xml:space="preserve"> CONCATENATE(CEILING(Table1[[#This Row],[Current Part/Page]]/Table1[[#This Row],[Part/Page count]], 0.0001) * 100,"%")</f>
+        <v>10%</v>
+      </c>
+      <c r="F38" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G38" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="H38" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="I38" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="J38" s="8"/>
+    </row>
+    <row r="39" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="8">
+        <v>35</v>
+      </c>
+      <c r="B39" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C39" s="8">
+        <v>200</v>
+      </c>
+      <c r="D39" s="8"/>
+      <c r="E39" s="10" t="str">
+        <f xml:space="preserve"> CONCATENATE(CEILING(Table1[[#This Row],[Current Part/Page]]/Table1[[#This Row],[Part/Page count]], 0.0001) * 100,"%")</f>
+        <v>0%</v>
+      </c>
+      <c r="F39" s="8"/>
+      <c r="G39" s="8"/>
+      <c r="H39" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="I39" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="J39" s="8"/>
+    </row>
+    <row r="40" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="8">
+        <v>36</v>
+      </c>
+      <c r="B40" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="C40" s="8">
+        <v>192</v>
+      </c>
+      <c r="D40" s="8">
+        <v>30</v>
+      </c>
+      <c r="E40" s="10" t="str">
+        <f xml:space="preserve"> CONCATENATE(CEILING(Table1[[#This Row],[Current Part/Page]]/Table1[[#This Row],[Part/Page count]], 0.0001) * 100,"%")</f>
+        <v>15.63%</v>
+      </c>
+      <c r="F40" s="8"/>
+      <c r="G40" s="8"/>
+      <c r="H40" s="9"/>
+      <c r="I40" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="J40" s="8"/>
+    </row>
+    <row r="41" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="8">
+        <v>37</v>
+      </c>
+      <c r="B41" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="C41" s="8">
+        <v>290</v>
+      </c>
+      <c r="D41" s="8">
+        <v>60</v>
+      </c>
+      <c r="E41" s="10" t="str">
+        <f xml:space="preserve"> CONCATENATE(CEILING(Table1[[#This Row],[Current Part/Page]]/Table1[[#This Row],[Part/Page count]], 0.0001) * 100,"%")</f>
+        <v>20.69%</v>
+      </c>
+      <c r="F41" s="8"/>
+      <c r="G41" s="8"/>
+      <c r="H41" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="I41" s="8"/>
+      <c r="J41" s="8"/>
+    </row>
+    <row r="42" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="8"/>
+      <c r="B42" s="8"/>
+      <c r="C42" s="8"/>
+      <c r="D42" s="8"/>
+      <c r="E42" s="10"/>
+      <c r="F42" s="8"/>
+      <c r="G42" s="8"/>
+      <c r="H42" s="8"/>
+      <c r="I42" s="8"/>
+      <c r="J42" s="8"/>
+    </row>
+    <row r="43" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="44" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="F1:I1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" copies="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
     <tablePart r:id="rId2"/>
   </tableParts>

</xml_diff>

<commit_message>
Doc: update the essay on education and schooling, update progress of english resources
</commit_message>
<xml_diff>
--- a/TOEFL/Progress.xlsx
+++ b/TOEFL/Progress.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="20895" yWindow="0" windowWidth="16980" windowHeight="8205"/>
+    <workbookView xWindow="22905" yWindow="0" windowWidth="16980" windowHeight="8205"/>
   </bookViews>
   <sheets>
     <sheet name="Progress" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="67">
   <si>
     <t>Book/CD Name</t>
   </si>
@@ -203,6 +203,24 @@
   </si>
   <si>
     <t>The American Accent</t>
+  </si>
+  <si>
+    <t>1000 Collocations</t>
+  </si>
+  <si>
+    <t>EngVid.com - Adam Courses</t>
+  </si>
+  <si>
+    <t>VOA - English In a Minute</t>
+  </si>
+  <si>
+    <t>EngVid.com - Resources</t>
+  </si>
+  <si>
+    <t>IELTS - Word Secret Band 9</t>
+  </si>
+  <si>
+    <t>IELTS - Academic and General Writing Task 2</t>
   </si>
 </sst>
 </file>
@@ -404,8 +422,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A2:J41" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18">
-  <autoFilter ref="A2:J41"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A2:J48" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18">
+  <autoFilter ref="A2:J48"/>
   <tableColumns count="10">
     <tableColumn id="1" name="No." dataDxfId="17"/>
     <tableColumn id="2" name="Book/CD Name" dataDxfId="16"/>
@@ -704,10 +722,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J44"/>
+  <dimension ref="A1:J58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B42" sqref="B42"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D42" sqref="D42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -984,7 +1002,9 @@
       <c r="J10" s="1"/>
     </row>
     <row r="11" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="8"/>
+      <c r="A11" s="8">
+        <v>9</v>
+      </c>
       <c r="B11" s="8" t="s">
         <v>58</v>
       </c>
@@ -1010,7 +1030,7 @@
     </row>
     <row r="12" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="8">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>43</v>
@@ -1036,15 +1056,22 @@
       <c r="J12" s="8"/>
     </row>
     <row r="13" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="8"/>
+      <c r="A13" s="8">
+        <v>11</v>
+      </c>
       <c r="B13" s="8" t="s">
         <v>59</v>
       </c>
       <c r="C13" s="8">
         <v>52</v>
       </c>
-      <c r="D13" s="8"/>
-      <c r="E13" s="10"/>
+      <c r="D13" s="8">
+        <v>28</v>
+      </c>
+      <c r="E13" s="10" t="str">
+        <f xml:space="preserve"> CONCATENATE(CEILING(Table1[[#This Row],[Current Part/Page]]/Table1[[#This Row],[Part/Page count]], 0.0001) * 100,"%")</f>
+        <v>53.85%</v>
+      </c>
       <c r="F13" s="8" t="s">
         <v>15</v>
       </c>
@@ -1057,7 +1084,7 @@
     </row>
     <row r="14" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="8">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>24</v>
@@ -1084,7 +1111,7 @@
     </row>
     <row r="15" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="8">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>18</v>
@@ -1107,7 +1134,7 @@
     </row>
     <row r="16" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="8">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B16" s="8" t="s">
         <v>27</v>
@@ -1138,7 +1165,7 @@
     </row>
     <row r="17" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="8">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B17" s="8" t="s">
         <v>28</v>
@@ -1167,7 +1194,7 @@
     </row>
     <row r="18" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="8">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B18" s="8" t="s">
         <v>29</v>
@@ -1196,7 +1223,7 @@
     </row>
     <row r="19" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="8">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B19" s="8" t="s">
         <v>30</v>
@@ -1225,7 +1252,7 @@
     </row>
     <row r="20" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="8">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B20" s="8" t="s">
         <v>32</v>
@@ -1254,7 +1281,7 @@
     </row>
     <row r="21" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="8">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B21" s="8" t="s">
         <v>33</v>
@@ -1283,7 +1310,7 @@
     </row>
     <row r="22" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="8">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B22" s="8" t="s">
         <v>34</v>
@@ -1312,7 +1339,7 @@
     </row>
     <row r="23" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="8">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B23" s="8" t="s">
         <v>35</v>
@@ -1341,7 +1368,7 @@
     </row>
     <row r="24" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="8">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B24" s="8" t="s">
         <v>36</v>
@@ -1372,7 +1399,7 @@
     </row>
     <row r="25" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="8">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B25" s="8" t="s">
         <v>37</v>
@@ -1403,7 +1430,7 @@
     </row>
     <row r="26" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="8">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B26" s="8" t="s">
         <v>38</v>
@@ -1432,7 +1459,7 @@
     </row>
     <row r="27" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="8">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B27" s="8" t="s">
         <v>39</v>
@@ -1461,7 +1488,7 @@
     </row>
     <row r="28" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="8">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B28" s="8" t="s">
         <v>31</v>
@@ -1490,7 +1517,7 @@
     </row>
     <row r="29" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="8">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B29" s="8" t="s">
         <v>42</v>
@@ -1519,7 +1546,7 @@
     </row>
     <row r="30" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="8">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B30" s="8" t="s">
         <v>45</v>
@@ -1548,7 +1575,7 @@
     </row>
     <row r="31" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="8">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B31" s="8" t="s">
         <v>48</v>
@@ -1577,7 +1604,7 @@
     </row>
     <row r="32" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="8">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B32" s="8" t="s">
         <v>47</v>
@@ -1606,7 +1633,7 @@
     </row>
     <row r="33" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="8">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B33" s="8" t="s">
         <v>49</v>
@@ -1639,7 +1666,7 @@
     </row>
     <row r="34" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="8">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B34" s="8" t="s">
         <v>50</v>
@@ -1666,7 +1693,7 @@
     </row>
     <row r="35" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="8">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B35" s="8" t="s">
         <v>51</v>
@@ -1699,7 +1726,7 @@
     </row>
     <row r="36" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="8">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B36" s="8" t="s">
         <v>54</v>
@@ -1730,7 +1757,7 @@
     </row>
     <row r="37" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="8">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B37" s="8" t="s">
         <v>55</v>
@@ -1759,7 +1786,7 @@
     </row>
     <row r="38" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="8">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B38" s="8" t="s">
         <v>56</v>
@@ -1790,7 +1817,7 @@
     </row>
     <row r="39" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="8">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B39" s="8" t="s">
         <v>23</v>
@@ -1815,7 +1842,7 @@
     </row>
     <row r="40" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="8">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B40" s="8" t="s">
         <v>57</v>
@@ -1824,11 +1851,11 @@
         <v>192</v>
       </c>
       <c r="D40" s="8">
-        <v>30</v>
+        <v>80</v>
       </c>
       <c r="E40" s="10" t="str">
         <f xml:space="preserve"> CONCATENATE(CEILING(Table1[[#This Row],[Current Part/Page]]/Table1[[#This Row],[Part/Page count]], 0.0001) * 100,"%")</f>
-        <v>15.63%</v>
+        <v>41.67%</v>
       </c>
       <c r="F40" s="8"/>
       <c r="G40" s="8"/>
@@ -1840,7 +1867,7 @@
     </row>
     <row r="41" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="8">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B41" s="8" t="s">
         <v>60</v>
@@ -1849,11 +1876,11 @@
         <v>290</v>
       </c>
       <c r="D41" s="8">
-        <v>60</v>
+        <v>290</v>
       </c>
       <c r="E41" s="10" t="str">
         <f xml:space="preserve"> CONCATENATE(CEILING(Table1[[#This Row],[Current Part/Page]]/Table1[[#This Row],[Part/Page count]], 0.0001) * 100,"%")</f>
-        <v>20.69%</v>
+        <v>100%</v>
       </c>
       <c r="F41" s="8"/>
       <c r="G41" s="8"/>
@@ -1864,19 +1891,198 @@
       <c r="J41" s="8"/>
     </row>
     <row r="42" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="8"/>
-      <c r="B42" s="8"/>
-      <c r="C42" s="8"/>
-      <c r="D42" s="8"/>
-      <c r="E42" s="10"/>
-      <c r="F42" s="8"/>
-      <c r="G42" s="8"/>
-      <c r="H42" s="8"/>
-      <c r="I42" s="8"/>
+      <c r="A42" s="8">
+        <v>40</v>
+      </c>
+      <c r="B42" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="C42" s="8">
+        <v>50</v>
+      </c>
+      <c r="D42" s="8">
+        <v>14</v>
+      </c>
+      <c r="E42" s="10" t="str">
+        <f xml:space="preserve"> CONCATENATE(CEILING(Table1[[#This Row],[Current Part/Page]]/Table1[[#This Row],[Part/Page count]], 0.0001) * 100,"%")</f>
+        <v>28%</v>
+      </c>
+      <c r="F42" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G42" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="H42" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="I42" s="9" t="s">
+        <v>15</v>
+      </c>
       <c r="J42" s="8"/>
     </row>
-    <row r="43" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="44" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="43" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="8">
+        <v>41</v>
+      </c>
+      <c r="B43" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="C43" s="8">
+        <v>144</v>
+      </c>
+      <c r="D43" s="8">
+        <v>18</v>
+      </c>
+      <c r="E43" s="10" t="str">
+        <f xml:space="preserve"> CONCATENATE(CEILING(Table1[[#This Row],[Current Part/Page]]/Table1[[#This Row],[Part/Page count]], 0.0001) * 100,"%")</f>
+        <v>12.5%</v>
+      </c>
+      <c r="F43" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G43" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="H43" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="I43" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="J43" s="8"/>
+    </row>
+    <row r="44" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="8">
+        <v>42</v>
+      </c>
+      <c r="B44" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="C44" s="8">
+        <v>100</v>
+      </c>
+      <c r="D44" s="8">
+        <v>1</v>
+      </c>
+      <c r="E44" s="10" t="str">
+        <f xml:space="preserve"> CONCATENATE(CEILING(Table1[[#This Row],[Current Part/Page]]/Table1[[#This Row],[Part/Page count]], 0.0001) * 100,"%")</f>
+        <v>1%</v>
+      </c>
+      <c r="F44" s="9"/>
+      <c r="G44" s="9"/>
+      <c r="H44" s="9"/>
+      <c r="I44" s="9"/>
+      <c r="J44" s="8"/>
+    </row>
+    <row r="45" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="8">
+        <v>43</v>
+      </c>
+      <c r="B45" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="C45" s="8">
+        <v>240</v>
+      </c>
+      <c r="D45" s="8">
+        <v>2</v>
+      </c>
+      <c r="E45" s="10" t="str">
+        <f xml:space="preserve"> CONCATENATE(CEILING(Table1[[#This Row],[Current Part/Page]]/Table1[[#This Row],[Part/Page count]], 0.0001) * 100,"%")</f>
+        <v>0.84%</v>
+      </c>
+      <c r="F45" s="9"/>
+      <c r="G45" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="H45" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="I45" s="9"/>
+      <c r="J45" s="8"/>
+    </row>
+    <row r="46" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="8">
+        <v>44</v>
+      </c>
+      <c r="B46" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="C46" s="8">
+        <v>10</v>
+      </c>
+      <c r="D46" s="8">
+        <v>3</v>
+      </c>
+      <c r="E46" s="10" t="str">
+        <f xml:space="preserve"> CONCATENATE(CEILING(Table1[[#This Row],[Current Part/Page]]/Table1[[#This Row],[Part/Page count]], 0.0001) * 100,"%")</f>
+        <v>30%</v>
+      </c>
+      <c r="F46" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G46" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="H46" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="I46" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="J46" s="8"/>
+    </row>
+    <row r="47" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="8">
+        <v>45</v>
+      </c>
+      <c r="B47" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="C47" s="8">
+        <v>68</v>
+      </c>
+      <c r="D47" s="8">
+        <v>68</v>
+      </c>
+      <c r="E47" s="10" t="str">
+        <f xml:space="preserve"> CONCATENATE(CEILING(Table1[[#This Row],[Current Part/Page]]/Table1[[#This Row],[Part/Page count]], 0.0001) * 100,"%")</f>
+        <v>100%</v>
+      </c>
+      <c r="F47" s="8"/>
+      <c r="G47" s="8"/>
+      <c r="H47" s="8"/>
+      <c r="I47" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="J47" s="8"/>
+    </row>
+    <row r="48" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="8"/>
+      <c r="B48" s="8"/>
+      <c r="C48" s="8"/>
+      <c r="D48" s="8"/>
+      <c r="E48" s="10" t="e">
+        <f xml:space="preserve"> CONCATENATE(CEILING(Table1[[#This Row],[Current Part/Page]]/Table1[[#This Row],[Part/Page count]], 0.0001) * 100,"%")</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F48" s="8"/>
+      <c r="G48" s="8"/>
+      <c r="H48" s="8"/>
+      <c r="I48" s="8"/>
+      <c r="J48" s="8"/>
+    </row>
+    <row r="49" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="50" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="51" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="52" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="53" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="54" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="55" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="56" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="57" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="58" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="F1:I1"/>

</xml_diff>